<commit_message>
Update questions and create new functions
</commit_message>
<xml_diff>
--- a/data/questions_dataset.xlsx
+++ b/data/questions_dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodrigoperes\Documents\codes\LLMs-IME_ITA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B1E912-ADD6-4498-B28C-ABD79D1496B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0B15AA-91F1-463D-9B0B-3102ACC3819E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="870" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2611,43 +2611,6 @@
 c) III.
 d) I e III.
 e) I e III.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tokens required
-Texto 1
-Erico Verissimo (1905 – 1975), nascido em Cruz Alta (RS), foi um dos escritores mais populares da chamada segunda fase modernista, que começou na década de 1930. Sua obra mais conhecida é o “Tempo e o Vento”, uma trilogia de romances, na qual ele narra a história de um clã familiar, os Terra Cambarás, de 1745 até 1945, tendo como contexto à formação da fronteira nacional na região sul. O espaço central desses romances é a cidade fictícia de Santa Fé, situada no noroeste do Rio Grande do Sul. O texto “O Sobrado”, que integra o romance “O Continente”, versa sobre o chefe do clã, Licurgo Cambará, que resiste em casa ao cerco dos inimigos pertencentes ao clã oposto, dos Amaral. Na obra, é abordado um episódio da Revolução Federalista (1893 – 1895), uma guerra civil entre dois grupos de ideias opostas: um que desejava aumentar os poderes do presidente da República e outro que desejava uma maior autonomia aos estados.
-O SOBRADO
-   Era uma noite fria de lua cheia. As estrelas cintilavam sobre a cidade de Santa Fé, que de tão quieta e deserta parecia um cemitério abandonado. Era tanto o silêncio e tão leve o ar, que se alguém aguçasse o ouvido talvez pudesse até escutar o sereno na solidão.
-   Agachado atras dum muro, José Lírio preparava-se para a última corrida. Quantos passos dali até a igreja? Talvez uns dez ou doze, bem puxados. Recebera ordens para revezar o companheiro que estava de vigia no alto duma das torres da Matriz. “Tenente Liroca”, dissera-lhe o coronel, havia poucos minutos, “suba pro alto do        campanário e fique de olho firme no quintal do Sobrado. Se alguém aparecer pra tirar água do poço, faça fogo sem piedade.”
-   José Lírio olhava a rua. Dez passos até a igreja. Mas quantos passos até a morte? Talvez cinco... ou dois. Havia um atirador infernal na água-furtada do Sobrado, à espreita dos imprudentes que se aventurassem a cruzar a praça ou alguma rua a descoberto.
-   Os segundos passavam. Era preciso cumprir a ordem. Liroca não queria que ninguám percebesse que ele hesitava, que era um covarde. Sim, covarde. Podia enganar os outros, mas nao conseguia iludir-se a si mesmo.
-   Estava metido naquela revolução porque era federalista e tinha vergonha na cara. Mas não se habituava nunca ao perigo. Sentira medo desde o primeiro dia, desde a primeira hora — um medo que lhe vinha de baixo das tripas, e lhe subia pelo estomago até a goela, como uma geada, amolecendo-lhe as pernas, os braços, a vontade. Medo é doença; medo é febre.
-   Engraçado. A noite estava fria mas o suor escorria-lhe pela cara barbuda e entrava-lhe na boca, com gosto de salmoura.
-   O tiroteio cessara ao entardecer. Talvez a munição da gente do Sobrado tivesse acabado. Ele podia atravessar a rua devagarinho, assobiando e acendendo um cigarro. Seria até uma provocação bonita. Vamos, Liroca, honra o lenço encarnado. Mas qual! Lá estava aquela sensação fria de vazio e enjoo na boca do estômago, o minuano gelado nos miúdos.
-   Donde lhe vinha tanto medo? Decerto do sangue da mãe, pois as gentes do lado paterno eram corajosas. O avô de Liroca fora um bravo em 35. O pai lhe morrera naquela mesma revolução, havia pouco mais dum ano tombara estripado numa carga de lança, mas lutando ate o último momento.
-   “Lírio é macho”, murmurou Liroca para si mesmo. “Lírio é macho.” Sempre que ia entrar num combate, repetia estas palavras: “Lírio é macho”.
-   Levantou-se devagarinho, apertando a carabina com ambas as maos. Sentia o corpo dorido, a garganta seca. Tornou a olhar para a igreja. Dez passos. Podia percorrê-los nuns cinco segundos, quando muito. Era só um upa e estava tudo terminado. Fez avançar cautelosamente a cabeça e, com a quina do muro a tocar-lhe o meio da testa e a ponta do nariz, fechou o olho direito e com o esquerdo ficou espiando o Sobrado que lá estava, do outro lado da praça, com sua fachada branca, a dupla fileira de janelas, a sacada de ferro e os altos muros de fortaleza. Havia no casarão algo de terrivelmente humano que fez o coração de José Lírio pulsar com mais força.
-   Os federalistas tinham tomado a cidade havia quase uma semana, mas Licurgo Cambara, o intendente e chefe político republicano do município, encastelara-se em sua casa com toda a família e um grupo de correligionários, e de lá ainda oferecia resistência. Enquanto o Sobrado não capitulasse, os revolucionários não poderiam considerar-se senhores de Santa Fé, pois os atiradores da água-furtada praticamente dominavam         a praça e as ruas em derredor.
-   Por alguns instantes José Lírio ficou a mirar a fachada do casarão, e de repente a lembrança de que Maria Valéria estava lá dentro lhe varou o peito como um pontaço de lança. Soltou um suspiro fundo e entrecortado, que foi quase um soluço. De novo se encolheu atrás do muro e tornou a olhar para a igreja. Se conseguisse chegar a salvo até a parede lateral, ficaria fora do alcance do atirador do Sobrado, e poderia entrar no campanário pela porta da sacristia.
-   Vamos, Liroca, so uma corrida. Que te pode acontecer? O homem te enxerga, faz pontaria, atira e acerta. Uma bala na cabeça. Pronto! Cais de cara no chão e está tudo liquidado. Acaba-se a agonia. Dizem que quando a bala entra no corpo da gente, no primeiro momento não dói. Depois é que vem a ardência, como se ela fosse de ferro em brasa. Mas quando o ferimento é mortal não se sente nada. O pior é arma branca. Vamos, Liroca. Dez passos. Cinco segundos. Lírio é macho, Lírio é macho.
-   José Lírio continuava imóvel, olhando a rua. Ainda ontem um companheiro seu ousara atravessar aquele trecho à luz do dia, num momento em que o tiroteio cessara. Ia cantando e fanfarronando. Viu-se de repente na água-furtada do sobrado um clarão acompanhado dum estampido, e o homem tombou. O sangue começou a borbotar-lhe do peito e a empapar a terra.
-   “Vamos, menino!” Quem falava agora nos pensamentos de Liroca era seu pai, o velho Maneco Lírio. Sua voz áspera como lixa vinha de longe, de um certo dia da infância em que Liroca faltara à escola e ao chegar a casa encontrara o pai atras da porta com um rebenque na mão. “Agora tu me pagas, salafrário!” Liroca saíra a correr como um doido na direc¸ao do fundo do quintal. “Espera, poltrão!” E de repente o que o velho Maneco tinha nas mãos não era mais o chicote, e sim as próprias vísceras, que lhe escorriam moles e visguentas da ferida do ventre. “Vamos, covarde!”
-   De súbito, como tomado dum demônio, Liroca ergueu-se, apertou a carabina contra o peito e deitou a correr na direção da igreja. Seus passos soaram fofos na terra. Deu cinco passadas e a meio caminho, sem olhar para o Sobrado, numa voz frenética de quem pede socorro, gritou: “Pica-paus do inferno! Sou homem!”. Continuou a correr e, ao chegar ao ponto morto atras da parede lateral da igreja, rojou-se ao solo e ali ficou, arquejante, com o peito colado à terra, o coração a bater acelerado, e sentindo entrar-lhe na boca e nas narinas talos de grama umida de sereno. “A la fresca!”, murmurou ele. “A la fresca!”
-   Estava inteiro, estava salvo. Fechou os olhos e deixou-se quedar onde estava, babujando a terra com sua saliva grossa, a garganta a arder, e o corpo todo amolentado por uma fraqueza que lhe dava um trêmulo desejo de chorar.
-VERISSIMO, Erico. O tempo e o vento, parte I: O Continente. 4ª ed. Sao Paulo: Companhia das Letras, 2013, p. 17- 19 (texto adaptado).
-Texto 2
-PENSAR A CIBERGUERRA
-   A ideia de ciberguerra tem sido questionada por alguns estudiosos, tanto militares quanto civis. Para Thomas Rid, por exemplo, não houve at é o momento qualquer ciberataque que possa enquadrar na clássica definição de Clausewitz¹ para o “ato de guerra”. Para o pensador prussiano, basicamente se pode classificar como ato de guerra algo relacionado a ações violentas. Além disso, o ato de guerra é sempre “instrumental”, isto é, através da violência física ou da ameaça do uso da força e possível impelir o inimigo a realizar aquilo que o atacante deseja. E ainda não se deve esquecer uma terceira característica do ato de guerra: o ataque deve ser algum tipo de ideia-noção ou intenção de meta política. Um dos problemas apresentados aqui e pensar aquilo que se entende por “violência”. Nesse caso, conforme Jarno Limnéll, estamos lidando com um conceito ambíguo, que agrega mais do que causas físicas ou a morte.
-   A ciberguerra compõe parte daquilo que alguns chamam de “guerra não convencional”. A ocorrência de um incidente envolvendo ataques à rede de um determinado país logo desperta comparações com a vasta filmografia sobre “revoltas de computadores”, sobre os indomavéis hackers. Mas, ao contrário, talvez fosse interessante diminuir os excessos sobre o assunto e trazê-lo cuidadosamente para o lugar da história. O texto “Cyberwar is coming!”, de John Arquilla e David Ronfeldt, foi um dos primeiros a apontar a singularidade de novos modos de conflito. Publicado pela Rand Corporation, agência reconhecida por subsidiar o Departamento de Defesa norte-americano, o trabalho da dupla repercutiu ao apresentar a necessidade de pensar as tecnologias da informação como aspecto central nas novas estratégias militares. Arquilla e Ronfeldt destacam a necessidade de conhecer o campo inimigo, revelam inspiração nos mongóis do século XIII, afirmam a importância de considerar a relação histórica entre mudanças tecnológicas e novas formulações para as doutrinas militares.
-   Anos depois, a mesma dupla de pesquisadores publicaria outro trabalho, procurando delimitar aquilo a que chamaram de netwar, a guerra em rede. Para eles, esse modo de conflito ganharia preponderancia, haja vista que, para levar adiante uma ciberguerra, seria necessaria uma quantidade maior de recursos financeiros e um repertorio menor de artefatos a serem utilizados. A netwar seria típica de conflitos de baixa intensidade, sendo perceptível com maior nitidez nas ações de grupos como o Hamas e os zapatistas.
-   Provavelmente, a diferença mais visível entre os dois tipos de conflito, ciberguerra e guerra em rede, possa        ser observada no fato de que o primeiro exige o uso de ambientes cibernéticos, enquanto o segundo não. Sendo assim, as ciberguerras apresentam um maior potencial para serem empreendidas por agentes estatais, embora isso não seja uma regra. Os formatos em torno da ciberguerra também evidenciam a necessidade do uso das redes de computadores para que os resultados esperados sejam atingidos.
-   Nye Jr. chama a atenção para a força que os conflitos cibernéticos ganharam neste século. O fato de possibilitarem a participação de agentes não estatais e a inserção cada vez mais profunda dos computadores e softwares na vida cotidiana somente reforça a necessidade de considerarmos os influxos desse tipo de ação. Evidentemente, acompanhar a ideia de que existe ciberguerra envolve a compreensao das semelhanças e diferenças em relação ao que classicamente consideramos uma guerra.
-   Numa guerra do tipo clássico, o aspecto físico exerce papel fundamental. Deve-se levar em conta o preparo de tropas fisicamente saudáveis, habilidosas no manejo de armamentos e com a possibilidade de movimentação em diferentes terrenos. Em tal modalidade de guerra, os combates tendem a cessar a partir da exaustão das tropas ou por seu desgaste. Por um lado, os governos dispõem de um quase monopólio do uso da força em larga escala, e os defensores precisam conhecer muito bem o terreno de movimentação. Além disso, é preciso considerar que um combate desse tipo requer consideráveis recursos de manutenção, mobilidade e investimentos financeiros. Afinal de contas, deslocar tropas do Atlântico Norte para o Pacífico ou da América do        Sul para a África exige tempo e considerável gasto com combustíveis, entre outros.
-   Toda essa situação ganha contornos diferentes na ciberguerra. Nela podem atuar diversos atores, estatais e não estatais, identificados e anônimos. A distância física e quase irrelevante, o ataque se sobrepõe a defesa, já que a rede mundial de computadores não foi pensada como algo a ser necessariamente defendido. Outra característica está no fato de que a parte maior, e oficialmente mais poderosa, tem capacidade limitada para desarmar ou destruir o inimigo, ocupar o território ou usar efetivamente estratégias de força contrária.
-   Em 2014, por exemplo, nos confrontos entre a Rússia e a Ucrânia, o sistema de comunicações via telefone celular ucraniano foi atacado. A companhia Ukrtelecom teve suas instalações invadidas por homens armados que danificaram cabos de fibra ótica, comprometendo seriamente o fornecimento do serviço. Por outro lado, grupos de hackers ucranianos, a exemplo do Cyber-Berkut, atacaram as páginas russas. O site da agência de comunicação estatal Russia Today foi invadido e nele a palavra “russos” foi substituída por “nazistas”. Justamente por suas características, trata-se de um conflito que mais frequentemente se desenvolve nas sombras, com certa discrição. Se há cibercomandos, eles são anunciados sempre como unidades de função defensiva, não de ataque. Ao mesmo tempo, é importante pensar que as intervenções cibernéticas podem servir como ato de abertura de uma guerra mais convencional. Dito de outro modo, um ataque cibernético pode ser o primeiro passo em uma ação maior.
-LEÃO, Kari; SILVA, Francisco. Por que a guerra?: Das batalhas gregas a ciberguerra - uma história da violência entre os homens. 1ª ed. Rio de Janeiro: Civilização Brasileira, 2018, p. 469 - 472 (texto adaptado).
-¹ Carl Von Clausewitz (1790 – 1831) – foi um experiente militar prussiano, especialista em estratégias de batalhas e considerado um grande teórico devido às suas definições amplamente difundidas sobre a guerra.
-</t>
   </si>
   <si>
     <t>“A ciberguerra compoe parte daquilo que alguns chamam de “guerra não convencional” [...]. Arquilla e Ronfeldt destacam a necessidade de conhecer o campo inimigo, revelam inspiração nos mongóis [...] para as doutrinas militares.” ´ (texto 2, linhas 10 a 20)
@@ -3685,50 +3648,6 @@
 e) I, II e III, apenas.</t>
   </si>
   <si>
-    <t>Tokens required
-Publicada em 1902, a partir de um trabalho de correspondente de guerra encomendado pelo jornal "A Província de São Paulo" ao engenheiro militar Euclides da Cunha, oriundo da Escola Militar da Praia Vermelha (atualmente, Instituto Militar de Engenharia), a obra "Os Sertões" aborda os acontecimentos da chamada guerra de Canudos, que foi o confronto entre um movimento popular missiânico e o Exército Nacional, de 1896 a 1897, no interior do estado da Bahia. Uma leitura obrigatória para a compreensão da sociedade e da cultura brasileira, a obra reflete a descoberta pelo autor de um "Brasil profundo", desconhecido pela elite intelectual e política do litoral, e se tornou obra canônica de expressão dos problemas e temas da nacionalidade. Em tom erudito, "Os Sertões" se caracteriza pelo encontro do estilo com os conceitos científicos, que são estetizados e transfigurados, para estabelecer um novo plano de realidade humana, por meio de uma escrita tortuosa, gramaticalmente rebuscada, marcada pela rica adjetivação e reinvenção lexical. 
-Texto 1 
-Capítulo 3 - A GUERRA DAS CAATINGAS
-   Os doutores na arte de matar que hoje, na Europa, invadem escandalosamente a ciência, perturbando-lhe o remanso com um retinir de esporas insolentes — e formulam leis para a guerra, pondo em equação as batalhas, têm definido bem o papel das florestas como agente tático precioso, de ofensiva ou defensiva. E ririam os sábios feldmarechais — guerreiros de cujas mãos caiu o franquisque heróico trocado pelo lápis calculista — se ouvissem a alguém que às caatingas pobres cabe função mais definida e grave que às grandes matas virgens. Porque estas, malgrado a sua importância para a defesa do território — orlando as fronteiras e quebrando o embate às invasões, impedindo mobilizações rápidas e impossibilitando a translação das artilharias — se tornam de algum modo neutras no curso das campanhas. Podem favorecer, indiferentemente, aos dois beligerantes oferecendo a ambos a mesma penumbra às emboscadas, dificultando-lhes por igual as manobras ou todos os desdobramentos em que a estratégia desencadeia os exércitos. São uma variável nas fórmulas do problema tenebroso da guerra, capaz dos mais opostos valores.
-   Ao passo que as caatingas são um aliado incorruptível do sertanejo em revolta. Entram também de certo modo na luta. Armam-se para o combate; agridem. Trançam-se, impenetráveis, ante o forasteiro, mas abrem-se em trilhas multívias, para o matuto que ali nasceu e cresceu.
-   E o jagunço faz-se o guerrilheiro-tugue, intangível...
-   As caatingas não o escondem apenas, amparam-no.
-   Ao avistá-las, no verão, uma coluna em marcha não se surpreende. Segue pelos caminhos em torcicolos, aforradamente. E os soldados, devassando com as vistas o matagal sem folhas, nem pensam no inimigo. Reagindo à canícula e com o desalinho natural às marchas, prosseguem envoltos no vozear confuso das conversas travadas em toda a linha, virguladas de tinidos de armas, cindidas de risos joviais mal sofreados.
-   É que nada pode assustá-los. Certo, se os adversários imprudentes com eles se afrontarem, serão varridos em momentos. Aqueles esgalhos far-se-ão em estilhas a um breve
-choque de espadas e não é crível que os gravetos finos quebrem o arranco das manobras prontas. E lá se vão, marchando, tranqüilamente heróicos...
-   De repente, pelos seus flancos, estoura, perto, um tiro...
-    A bala passa, rechinante, ou estende, morto, em terra, um homem. Sucedem-se, pausadas, outras, passando sobre as tropas, em sibilos longos. Cem, duzentos olhos, mil olhos
-perscrutadores, volvem-se, impacientes, em roda. Nada vêem. 
-   Há a primeira surpresa. Um fluxo de espanto corre de uma a outra ponta das fileiras.
-   E os tiros continuam raros, mas insistentes e compassados, pela esquerda, pela direita, pela frente agora, irrompendo de toda a banda.
-   Então estranha ansiedade invade os mais provados valentes, ante o antagonista que vê e não é visto. Forma-se celeremente em atiradores uma companhia, mal destacada da massa de batalhões constritos na vareda estreita. Distende-se pela orla da caatinga. Ouve-se uma voz de comando; e um turbilhão de balas rola estrugidoramente dentro das galhadas...
-   Mas constantes, longamente intervalados sempre, zunem os projéteis dos atiradores invisíveis batendo em cheio nas fileiras.
-    A situação rapidamente engravesce, exigindo resoluções enérgicas. Destacam-se outras unidades combatentes, escalonando-se por toda a extensão do caminho, prontas à primeira voz; — e o comandante resolve carregar contra o desconhecido. Carrega-se contra os duendes. A força, de baionetas caladas, rompe, impetuosa, o matagal numa expansão irradiante de cargas. Avança com rapidez. Os adversários parecem recuar apenas. Nesse momento surge o antagonismo formidável da caatinga.
-   As seções precipitam-se para os pontos onde estalam os estampidos e estacam ante uma barreira flexível, mas impenetrável, de juremas. Enredam-se no cipoal que as agrilhoa, que Ihes arrebata das mãos as armas, e não vingam transpô-lo. Contornam-no. Volvem aos lados. Vê-se um como rastilho de queimada: uma linha de baionetas enfiando pelos gravetos secos. Lampeja por momentos entre os raios do sol joeirados pelas árvores sem folhas; e parte-se, faiscando, adiante, dispersa, batendo contra espessos renques de xiquexiques, unidos como quadrados cheios, de falanges, intransponíveis, fervilhando espinhos...
-   Circuitam-nos, estonteadamente, os soldados. Espalham-se, correm à toa, num labirinto de galhos. Caem, presos pelos laços corredios dos quipás reptantes; ou estacam, pernas
-imobilizadas por fortíssimos tentáculos. Debatem-se desesperadamente até deixarem em pedaços as fardas, entre as garras felinas de acúleos recurvos das macambiras...
-   Impotentes estadeiam, imprecando, o desapontamento e a raiva, agitando-se furiosos e inúteis. Por fim a ordem dispersa do combate faz-se a dispersão do tumulto. Atiram a esmo, sem pontaria, numa indisciplina de fogo que vitima os próprios companheiros. Seguem reforços. Os mesmos transes reproduzem-se maiores, acrescidas a confusão e a desordem; —enquanto em torno, circulando-os, rítmicos, fulminantes, seguros, terríveis, bem apontados, caem inflexivelmente os projetis tio adversário.
-   De repente cessam. Desaparece o inimigo que ninguém viu.
-   As seções voltam desfalcadas para a coluna, depois de inúteis pesquisas nas macegas. E voltam como se saíssem de recontro braço a braço, com selvagens: vestes em tiras; armas
-estrondadas ou perdidas; golpeados de gilvazes; claudicando, estropiados; mal reprimindo o doer infernal das folhas urticantes; frechados de espinhos.... .
-   A luta é desigual. A força militar decai a um plano interior Batem-na o homem e a terra. E quando o sertão estua nos bochornos dos estios longos não é difícil prever a quem cabe a vitória. Enquanto o minotauro, impotente e possante, inerme com a sua envergadura de aço e grifos de baionetas, sente a garganta exsicar-se-lhe de sede e, aos primeiros sintomas da fome, reflui à retaguarda, fugindo ante o deserto ameaçador e estéril, aquela flora agressiva abre ao sertanejo um seio carinhoso e amigo.
-(...) 
-   A natureza toda protege o sertanejo. Talha-o como Anteu, indomável. É um titã bronzeado fazendo vacilar a marcha dos exércitos.
-CUNHA, Euclides da. Os Sertões (Campanha de Canudos). 2ª ed. São Paulo: Editora Ciranda Cultural, 2018. p. 181-186.
-Texto 2
-ESTADOS DE VIOLÊNCIA 
-   A Guerra, na longa história dos homens, terá tido seus atores e suas cenas, seus heróis e seus espaços. seus personagens e seus teatros. Diversidade incrível das fardas, dos costumes, enfeites, armaduras, equipamentos. Multiplicidade dos terrenos: barro espesso ou poeira asfixiante, brejos viscosos, desfiladeiros rochosos, prados gordurentos ou panícies sombrias, colinas acidentadas, montanhas dentadas, muros grossos das cidades fortificadas, portões e fossos profundos. Sem mesmo falar das táticas de combate, da evolução técnica das armas.
-   Mas o que malgrado tudo ficaria e basearia a distinção entre guerras maiores e menores, grandes e pequenas, verdadeiras e degradadas, era essa forma pura de fois exércitos engajando forças representando entidades políticas identificáveis, afrontando-se em batalhas decisivas, terrestres ou marítimas, que os colocavam em contato com seu princípio de encerramento: vitória ou derrota. É ainda possível essa forma pura de guerra, depois que as grandes e principais potências dispõem da arma absoluta (o fogo nuclear), depois ainda que um sí possui uma superioridade arrasadora das forças clássicas de destruição, tecnologias de reconhecimento, técnicas de fundição de precisão, depois enfim que as democracias desenvolveram uma cultura de negociação, de arbitragem em que o recurso à força nua é dado como inadequado, selvagem, contraproducente? Imagina-se que no futuro ainda grandes potências mobilizem o conjunto de suas forças vivas para se medirem? 
-   Na trama visível, dilacerada das grandes guerras contemporâneas, reconhecem-se apenas a paisagem cultural da guerra, as nervuras de sua representação dominante. Não se veem mais, e tanto melhor, colunas de soldados em centenas de milhares chegando ao futuro campo de batalha, dispondo-se em ordem para a batalha decisiva. Não se espera mais com um entusiasmo ansioso a sanção das armas: duração da batalha, data de vitória ou da derrota (...) Os estados de violência fazem aparecer uma multiplicidade de figuras novas: o terrorista, o chefe de facções, o mercenário, o soldado profissional, o engenheiro de informática, o responsável da segurança etc. Não exército disciplinado, mas redes dispersas, concorrentes, profissionais da violência. Mudanças ainda no nível do teatro dos conflitos. Para a guerra: uma planície, espaços largos, às vezes colinas ou rios, em todo caso campanhas (para não levar em conta aqui guerras de cerco). E depois vem o espetáculo desolador após a batalha: os inimigos como que abraçados na morte,
-corpos juncando o solo, fardas rasgadas, manchas de sangue. Um grande silêncio depois de tantos gritos e de vaias. O novo teatro é hoje a cidade. Não a cidade fortificada, em torno da qual se entrincheira, mas a cidade viva dos transeuntes. A dos espaços públicos: mercados, garagens, terraços de café, metrôs... A das ruas que francos atiradores isolados transformam em teatro de feira para divertimentos atrozes (...)
-   Tempos e espaços, personagens e cadáveres. Aqui se trata apenas do regime de imagens de violência armada que se acha transformado. A aposta filosófica sera dizer que acontece outra coisa, e não a guerra, que se poderia chamar provisoriamente de "estado de violência", porque eles se oporiam ao que os clássicos tinham definido como "estado de guerra" e também como "estado de natureza" (...)
-   Diante da inquietante extravagância desses conflitos dificilmente identificáveis ou codificáveis nos quadros da análise estratégica clássica, ouve-se mesmo: o pior estava por vir. 
-É preciso dizer que a polemologia (estudo da guerra) não reconhece mais seus filhos: nem seus chefes responsáveis, nem seus soldados dóceis, nem seus heróis esplêndidos, nem seus mortos no campo de honra. Chega-se mesmo a se queixar. Neste ponto, contudo, a nostalgia é dificilmente suportável. Sobretutdo para lastimar guerras que às vezes nem mesmo foram vividas pessoalmente. Estas boas velhas guerras, com bons velhos inimigos, fomentadas por Estados, alegando "razões", deve-se recordar que foram também o instrumento das mais baixas ambições, das mais loucas pretensões, dos mais sórdidos cálculos? Que elas acarretaram sem falhar o sacrifício de milhões de homens que não pediam senão para viver, que elas esgotaram precocemente civilizações desenvolvidas, conduziram culturas prestigiosas ao suicídio?
-   Resta, além de um pensamento nostálgico, compreender o que causa os estados atuais de violência. Então, antes que falar da "nova guerra", de "guerra selvagem", "guerra sem a
-guerra", de "guerra sem fim", de "guerra assimétrica", de "guerra civil generalizada", de "guerra ruiva", é preciso elucidar, em lugar do jogo antigo da guerra e da paz, as estruturações destes estados de violência (...) Como a filosofia clássica tinha conceituado o estado de guerra e de natureza, seria preciso esboçar a análise filosófica dos estados de violência, como distrubuição contemporânea das forças de destruição. 
-GROS, Frédéric. Estados de violência: ensaio sobre o fim da guerra. Tradução de José Augusto da Silva. Aparecida, SP. Editora Ideias &amp; Letras, 2009. p. 227-232 (texto adaptado).</t>
-  </si>
-  <si>
     <t>Comparando os Textos 1 e 2 em relação aos tipos textuais, é correto afirmar que</t>
   </si>
   <si>
@@ -5463,6 +5382,85 @@
 d) Incorreta. Nesse caso, o termo separado por vírgulas é uma oração de valor adverbial, e não está deslocada de sua posição sintática canônica; 
 e) Correta. A expressão “diante da inquietante extravagância…” tem papel adverbial e está topicalizada, deslocada de sua posição original, como no exemplo.
 A resposta correta então é a letra e) “**Diante da inquietante extravagância desses conflitos dificilmente identificáveis ou codificáveis nos quadros da análise estratégica clássica**, ouve-se mesmo o pior estaria por vir” (Texto 2, linhas 39 e 40).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Texto 1
+Erico Verissimo (1905 – 1975), nascido em Cruz Alta (RS), foi um dos escritores mais populares da chamada segunda fase modernista, que começou na década de 1930. Sua obra mais conhecida é o “Tempo e o Vento”, uma trilogia de romances, na qual ele narra a história de um clã familiar, os Terra Cambarás, de 1745 até 1945, tendo como contexto à formação da fronteira nacional na região sul. O espaço central desses romances é a cidade fictícia de Santa Fé, situada no noroeste do Rio Grande do Sul. O texto “O Sobrado”, que integra o romance “O Continente”, versa sobre o chefe do clã, Licurgo Cambará, que resiste em casa ao cerco dos inimigos pertencentes ao clã oposto, dos Amaral. Na obra, é abordado um episódio da Revolução Federalista (1893 – 1895), uma guerra civil entre dois grupos de ideias opostas: um que desejava aumentar os poderes do presidente da República e outro que desejava uma maior autonomia aos estados.
+O SOBRADO
+   Era uma noite fria de lua cheia. As estrelas cintilavam sobre a cidade de Santa Fé, que de tão quieta e deserta parecia um cemitério abandonado. Era tanto o silêncio e tão leve o ar, que se alguém aguçasse o ouvido talvez pudesse até escutar o sereno na solidão.
+   Agachado atras dum muro, José Lírio preparava-se para a última corrida. Quantos passos dali até a igreja? Talvez uns dez ou doze, bem puxados. Recebera ordens para revezar o companheiro que estava de vigia no alto duma das torres da Matriz. “Tenente Liroca”, dissera-lhe o coronel, havia poucos minutos, “suba pro alto do        campanário e fique de olho firme no quintal do Sobrado. Se alguém aparecer pra tirar água do poço, faça fogo sem piedade.”
+   José Lírio olhava a rua. Dez passos até a igreja. Mas quantos passos até a morte? Talvez cinco... ou dois. Havia um atirador infernal na água-furtada do Sobrado, à espreita dos imprudentes que se aventurassem a cruzar a praça ou alguma rua a descoberto.
+   Os segundos passavam. Era preciso cumprir a ordem. Liroca não queria que ninguám percebesse que ele hesitava, que era um covarde. Sim, covarde. Podia enganar os outros, mas nao conseguia iludir-se a si mesmo.
+   Estava metido naquela revolução porque era federalista e tinha vergonha na cara. Mas não se habituava nunca ao perigo. Sentira medo desde o primeiro dia, desde a primeira hora — um medo que lhe vinha de baixo das tripas, e lhe subia pelo estomago até a goela, como uma geada, amolecendo-lhe as pernas, os braços, a vontade. Medo é doença; medo é febre.
+   Engraçado. A noite estava fria mas o suor escorria-lhe pela cara barbuda e entrava-lhe na boca, com gosto de salmoura.
+   O tiroteio cessara ao entardecer. Talvez a munição da gente do Sobrado tivesse acabado. Ele podia atravessar a rua devagarinho, assobiando e acendendo um cigarro. Seria até uma provocação bonita. Vamos, Liroca, honra o lenço encarnado. Mas qual! Lá estava aquela sensação fria de vazio e enjoo na boca do estômago, o minuano gelado nos miúdos.
+   Donde lhe vinha tanto medo? Decerto do sangue da mãe, pois as gentes do lado paterno eram corajosas. O avô de Liroca fora um bravo em 35. O pai lhe morrera naquela mesma revolução, havia pouco mais dum ano tombara estripado numa carga de lança, mas lutando ate o último momento.
+   “Lírio é macho”, murmurou Liroca para si mesmo. “Lírio é macho.” Sempre que ia entrar num combate, repetia estas palavras: “Lírio é macho”.
+   Levantou-se devagarinho, apertando a carabina com ambas as maos. Sentia o corpo dorido, a garganta seca. Tornou a olhar para a igreja. Dez passos. Podia percorrê-los nuns cinco segundos, quando muito. Era só um upa e estava tudo terminado. Fez avançar cautelosamente a cabeça e, com a quina do muro a tocar-lhe o meio da testa e a ponta do nariz, fechou o olho direito e com o esquerdo ficou espiando o Sobrado que lá estava, do outro lado da praça, com sua fachada branca, a dupla fileira de janelas, a sacada de ferro e os altos muros de fortaleza. Havia no casarão algo de terrivelmente humano que fez o coração de José Lírio pulsar com mais força.
+   Os federalistas tinham tomado a cidade havia quase uma semana, mas Licurgo Cambara, o intendente e chefe político republicano do município, encastelara-se em sua casa com toda a família e um grupo de correligionários, e de lá ainda oferecia resistência. Enquanto o Sobrado não capitulasse, os revolucionários não poderiam considerar-se senhores de Santa Fé, pois os atiradores da água-furtada praticamente dominavam         a praça e as ruas em derredor.
+   Por alguns instantes José Lírio ficou a mirar a fachada do casarão, e de repente a lembrança de que Maria Valéria estava lá dentro lhe varou o peito como um pontaço de lança. Soltou um suspiro fundo e entrecortado, que foi quase um soluço. De novo se encolheu atrás do muro e tornou a olhar para a igreja. Se conseguisse chegar a salvo até a parede lateral, ficaria fora do alcance do atirador do Sobrado, e poderia entrar no campanário pela porta da sacristia.
+   Vamos, Liroca, so uma corrida. Que te pode acontecer? O homem te enxerga, faz pontaria, atira e acerta. Uma bala na cabeça. Pronto! Cais de cara no chão e está tudo liquidado. Acaba-se a agonia. Dizem que quando a bala entra no corpo da gente, no primeiro momento não dói. Depois é que vem a ardência, como se ela fosse de ferro em brasa. Mas quando o ferimento é mortal não se sente nada. O pior é arma branca. Vamos, Liroca. Dez passos. Cinco segundos. Lírio é macho, Lírio é macho.
+   José Lírio continuava imóvel, olhando a rua. Ainda ontem um companheiro seu ousara atravessar aquele trecho à luz do dia, num momento em que o tiroteio cessara. Ia cantando e fanfarronando. Viu-se de repente na água-furtada do sobrado um clarão acompanhado dum estampido, e o homem tombou. O sangue começou a borbotar-lhe do peito e a empapar a terra.
+   “Vamos, menino!” Quem falava agora nos pensamentos de Liroca era seu pai, o velho Maneco Lírio. Sua voz áspera como lixa vinha de longe, de um certo dia da infância em que Liroca faltara à escola e ao chegar a casa encontrara o pai atras da porta com um rebenque na mão. “Agora tu me pagas, salafrário!” Liroca saíra a correr como um doido na direc¸ao do fundo do quintal. “Espera, poltrão!” E de repente o que o velho Maneco tinha nas mãos não era mais o chicote, e sim as próprias vísceras, que lhe escorriam moles e visguentas da ferida do ventre. “Vamos, covarde!”
+   De súbito, como tomado dum demônio, Liroca ergueu-se, apertou a carabina contra o peito e deitou a correr na direção da igreja. Seus passos soaram fofos na terra. Deu cinco passadas e a meio caminho, sem olhar para o Sobrado, numa voz frenética de quem pede socorro, gritou: “Pica-paus do inferno! Sou homem!”. Continuou a correr e, ao chegar ao ponto morto atras da parede lateral da igreja, rojou-se ao solo e ali ficou, arquejante, com o peito colado à terra, o coração a bater acelerado, e sentindo entrar-lhe na boca e nas narinas talos de grama umida de sereno. “A la fresca!”, murmurou ele. “A la fresca!”
+   Estava inteiro, estava salvo. Fechou os olhos e deixou-se quedar onde estava, babujando a terra com sua saliva grossa, a garganta a arder, e o corpo todo amolentado por uma fraqueza que lhe dava um trêmulo desejo de chorar.
+VERISSIMO, Erico. O tempo e o vento, parte I: O Continente. 4ª ed. Sao Paulo: Companhia das Letras, 2013, p. 17- 19 (texto adaptado).
+Texto 2
+PENSAR A CIBERGUERRA
+   A ideia de ciberguerra tem sido questionada por alguns estudiosos, tanto militares quanto civis. Para Thomas Rid, por exemplo, não houve at é o momento qualquer ciberataque que possa enquadrar na clássica definição de Clausewitz¹ para o “ato de guerra”. Para o pensador prussiano, basicamente se pode classificar como ato de guerra algo relacionado a ações violentas. Além disso, o ato de guerra é sempre “instrumental”, isto é, através da violência física ou da ameaça do uso da força e possível impelir o inimigo a realizar aquilo que o atacante deseja. E ainda não se deve esquecer uma terceira característica do ato de guerra: o ataque deve ser algum tipo de ideia-noção ou intenção de meta política. Um dos problemas apresentados aqui e pensar aquilo que se entende por “violência”. Nesse caso, conforme Jarno Limnéll, estamos lidando com um conceito ambíguo, que agrega mais do que causas físicas ou a morte.
+   A ciberguerra compõe parte daquilo que alguns chamam de “guerra não convencional”. A ocorrência de um incidente envolvendo ataques à rede de um determinado país logo desperta comparações com a vasta filmografia sobre “revoltas de computadores”, sobre os indomavéis hackers. Mas, ao contrário, talvez fosse interessante diminuir os excessos sobre o assunto e trazê-lo cuidadosamente para o lugar da história. O texto “Cyberwar is coming!”, de John Arquilla e David Ronfeldt, foi um dos primeiros a apontar a singularidade de novos modos de conflito. Publicado pela Rand Corporation, agência reconhecida por subsidiar o Departamento de Defesa norte-americano, o trabalho da dupla repercutiu ao apresentar a necessidade de pensar as tecnologias da informação como aspecto central nas novas estratégias militares. Arquilla e Ronfeldt destacam a necessidade de conhecer o campo inimigo, revelam inspiração nos mongóis do século XIII, afirmam a importância de considerar a relação histórica entre mudanças tecnológicas e novas formulações para as doutrinas militares.
+   Anos depois, a mesma dupla de pesquisadores publicaria outro trabalho, procurando delimitar aquilo a que chamaram de netwar, a guerra em rede. Para eles, esse modo de conflito ganharia preponderancia, haja vista que, para levar adiante uma ciberguerra, seria necessaria uma quantidade maior de recursos financeiros e um repertorio menor de artefatos a serem utilizados. A netwar seria típica de conflitos de baixa intensidade, sendo perceptível com maior nitidez nas ações de grupos como o Hamas e os zapatistas.
+   Provavelmente, a diferença mais visível entre os dois tipos de conflito, ciberguerra e guerra em rede, possa        ser observada no fato de que o primeiro exige o uso de ambientes cibernéticos, enquanto o segundo não. Sendo assim, as ciberguerras apresentam um maior potencial para serem empreendidas por agentes estatais, embora isso não seja uma regra. Os formatos em torno da ciberguerra também evidenciam a necessidade do uso das redes de computadores para que os resultados esperados sejam atingidos.
+   Nye Jr. chama a atenção para a força que os conflitos cibernéticos ganharam neste século. O fato de possibilitarem a participação de agentes não estatais e a inserção cada vez mais profunda dos computadores e softwares na vida cotidiana somente reforça a necessidade de considerarmos os influxos desse tipo de ação. Evidentemente, acompanhar a ideia de que existe ciberguerra envolve a compreensao das semelhanças e diferenças em relação ao que classicamente consideramos uma guerra.
+   Numa guerra do tipo clássico, o aspecto físico exerce papel fundamental. Deve-se levar em conta o preparo de tropas fisicamente saudáveis, habilidosas no manejo de armamentos e com a possibilidade de movimentação em diferentes terrenos. Em tal modalidade de guerra, os combates tendem a cessar a partir da exaustão das tropas ou por seu desgaste. Por um lado, os governos dispõem de um quase monopólio do uso da força em larga escala, e os defensores precisam conhecer muito bem o terreno de movimentação. Além disso, é preciso considerar que um combate desse tipo requer consideráveis recursos de manutenção, mobilidade e investimentos financeiros. Afinal de contas, deslocar tropas do Atlântico Norte para o Pacífico ou da América do        Sul para a África exige tempo e considerável gasto com combustíveis, entre outros.
+   Toda essa situação ganha contornos diferentes na ciberguerra. Nela podem atuar diversos atores, estatais e não estatais, identificados e anônimos. A distância física e quase irrelevante, o ataque se sobrepõe a defesa, já que a rede mundial de computadores não foi pensada como algo a ser necessariamente defendido. Outra característica está no fato de que a parte maior, e oficialmente mais poderosa, tem capacidade limitada para desarmar ou destruir o inimigo, ocupar o território ou usar efetivamente estratégias de força contrária.
+   Em 2014, por exemplo, nos confrontos entre a Rússia e a Ucrânia, o sistema de comunicações via telefone celular ucraniano foi atacado. A companhia Ukrtelecom teve suas instalações invadidas por homens armados que danificaram cabos de fibra ótica, comprometendo seriamente o fornecimento do serviço. Por outro lado, grupos de hackers ucranianos, a exemplo do Cyber-Berkut, atacaram as páginas russas. O site da agência de comunicação estatal Russia Today foi invadido e nele a palavra “russos” foi substituída por “nazistas”. Justamente por suas características, trata-se de um conflito que mais frequentemente se desenvolve nas sombras, com certa discrição. Se há cibercomandos, eles são anunciados sempre como unidades de função defensiva, não de ataque. Ao mesmo tempo, é importante pensar que as intervenções cibernéticas podem servir como ato de abertura de uma guerra mais convencional. Dito de outro modo, um ataque cibernético pode ser o primeiro passo em uma ação maior.
+LEÃO, Kari; SILVA, Francisco. Por que a guerra?: Das batalhas gregas a ciberguerra - uma história da violência entre os homens. 1ª ed. Rio de Janeiro: Civilização Brasileira, 2018, p. 469 - 472 (texto adaptado).
+¹ Carl Von Clausewitz (1790 – 1831) – foi um experiente militar prussiano, especialista em estratégias de batalhas e considerado um grande teórico devido às suas definições amplamente difundidas sobre a guerra.
+</t>
+  </si>
+  <si>
+    <t>Publicada em 1902, a partir de um trabalho de correspondente de guerra encomendado pelo jornal "A Província de São Paulo" ao engenheiro militar Euclides da Cunha, oriundo da Escola Militar da Praia Vermelha (atualmente, Instituto Militar de Engenharia), a obra "Os Sertões" aborda os acontecimentos da chamada guerra de Canudos, que foi o confronto entre um movimento popular missiânico e o Exército Nacional, de 1896 a 1897, no interior do estado da Bahia. Uma leitura obrigatória para a compreensão da sociedade e da cultura brasileira, a obra reflete a descoberta pelo autor de um "Brasil profundo", desconhecido pela elite intelectual e política do litoral, e se tornou obra canônica de expressão dos problemas e temas da nacionalidade. Em tom erudito, "Os Sertões" se caracteriza pelo encontro do estilo com os conceitos científicos, que são estetizados e transfigurados, para estabelecer um novo plano de realidade humana, por meio de uma escrita tortuosa, gramaticalmente rebuscada, marcada pela rica adjetivação e reinvenção lexical. 
+Texto 1 
+Capítulo 3 - A GUERRA DAS CAATINGAS
+   Os doutores na arte de matar que hoje, na Europa, invadem escandalosamente a ciência, perturbando-lhe o remanso com um retinir de esporas insolentes — e formulam leis para a guerra, pondo em equação as batalhas, têm definido bem o papel das florestas como agente tático precioso, de ofensiva ou defensiva. E ririam os sábios feldmarechais — guerreiros de cujas mãos caiu o franquisque heróico trocado pelo lápis calculista — se ouvissem a alguém que às caatingas pobres cabe função mais definida e grave que às grandes matas virgens. Porque estas, malgrado a sua importância para a defesa do território — orlando as fronteiras e quebrando o embate às invasões, impedindo mobilizações rápidas e impossibilitando a translação das artilharias — se tornam de algum modo neutras no curso das campanhas. Podem favorecer, indiferentemente, aos dois beligerantes oferecendo a ambos a mesma penumbra às emboscadas, dificultando-lhes por igual as manobras ou todos os desdobramentos em que a estratégia desencadeia os exércitos. São uma variável nas fórmulas do problema tenebroso da guerra, capaz dos mais opostos valores.
+   Ao passo que as caatingas são um aliado incorruptível do sertanejo em revolta. Entram também de certo modo na luta. Armam-se para o combate; agridem. Trançam-se, impenetráveis, ante o forasteiro, mas abrem-se em trilhas multívias, para o matuto que ali nasceu e cresceu.
+   E o jagunço faz-se o guerrilheiro-tugue, intangível...
+   As caatingas não o escondem apenas, amparam-no.
+   Ao avistá-las, no verão, uma coluna em marcha não se surpreende. Segue pelos caminhos em torcicolos, aforradamente. E os soldados, devassando com as vistas o matagal sem folhas, nem pensam no inimigo. Reagindo à canícula e com o desalinho natural às marchas, prosseguem envoltos no vozear confuso das conversas travadas em toda a linha, virguladas de tinidos de armas, cindidas de risos joviais mal sofreados.
+   É que nada pode assustá-los. Certo, se os adversários imprudentes com eles se afrontarem, serão varridos em momentos. Aqueles esgalhos far-se-ão em estilhas a um breve
+choque de espadas e não é crível que os gravetos finos quebrem o arranco das manobras prontas. E lá se vão, marchando, tranqüilamente heróicos...
+   De repente, pelos seus flancos, estoura, perto, um tiro...
+    A bala passa, rechinante, ou estende, morto, em terra, um homem. Sucedem-se, pausadas, outras, passando sobre as tropas, em sibilos longos. Cem, duzentos olhos, mil olhos
+perscrutadores, volvem-se, impacientes, em roda. Nada vêem. 
+   Há a primeira surpresa. Um fluxo de espanto corre de uma a outra ponta das fileiras.
+   E os tiros continuam raros, mas insistentes e compassados, pela esquerda, pela direita, pela frente agora, irrompendo de toda a banda.
+   Então estranha ansiedade invade os mais provados valentes, ante o antagonista que vê e não é visto. Forma-se celeremente em atiradores uma companhia, mal destacada da massa de batalhões constritos na vareda estreita. Distende-se pela orla da caatinga. Ouve-se uma voz de comando; e um turbilhão de balas rola estrugidoramente dentro das galhadas...
+   Mas constantes, longamente intervalados sempre, zunem os projéteis dos atiradores invisíveis batendo em cheio nas fileiras.
+    A situação rapidamente engravesce, exigindo resoluções enérgicas. Destacam-se outras unidades combatentes, escalonando-se por toda a extensão do caminho, prontas à primeira voz; — e o comandante resolve carregar contra o desconhecido. Carrega-se contra os duendes. A força, de baionetas caladas, rompe, impetuosa, o matagal numa expansão irradiante de cargas. Avança com rapidez. Os adversários parecem recuar apenas. Nesse momento surge o antagonismo formidável da caatinga.
+   As seções precipitam-se para os pontos onde estalam os estampidos e estacam ante uma barreira flexível, mas impenetrável, de juremas. Enredam-se no cipoal que as agrilhoa, que Ihes arrebata das mãos as armas, e não vingam transpô-lo. Contornam-no. Volvem aos lados. Vê-se um como rastilho de queimada: uma linha de baionetas enfiando pelos gravetos secos. Lampeja por momentos entre os raios do sol joeirados pelas árvores sem folhas; e parte-se, faiscando, adiante, dispersa, batendo contra espessos renques de xiquexiques, unidos como quadrados cheios, de falanges, intransponíveis, fervilhando espinhos...
+   Circuitam-nos, estonteadamente, os soldados. Espalham-se, correm à toa, num labirinto de galhos. Caem, presos pelos laços corredios dos quipás reptantes; ou estacam, pernas
+imobilizadas por fortíssimos tentáculos. Debatem-se desesperadamente até deixarem em pedaços as fardas, entre as garras felinas de acúleos recurvos das macambiras...
+   Impotentes estadeiam, imprecando, o desapontamento e a raiva, agitando-se furiosos e inúteis. Por fim a ordem dispersa do combate faz-se a dispersão do tumulto. Atiram a esmo, sem pontaria, numa indisciplina de fogo que vitima os próprios companheiros. Seguem reforços. Os mesmos transes reproduzem-se maiores, acrescidas a confusão e a desordem; —enquanto em torno, circulando-os, rítmicos, fulminantes, seguros, terríveis, bem apontados, caem inflexivelmente os projetis tio adversário.
+   De repente cessam. Desaparece o inimigo que ninguém viu.
+   As seções voltam desfalcadas para a coluna, depois de inúteis pesquisas nas macegas. E voltam como se saíssem de recontro braço a braço, com selvagens: vestes em tiras; armas
+estrondadas ou perdidas; golpeados de gilvazes; claudicando, estropiados; mal reprimindo o doer infernal das folhas urticantes; frechados de espinhos.... .
+   A luta é desigual. A força militar decai a um plano interior Batem-na o homem e a terra. E quando o sertão estua nos bochornos dos estios longos não é difícil prever a quem cabe a vitória. Enquanto o minotauro, impotente e possante, inerme com a sua envergadura de aço e grifos de baionetas, sente a garganta exsicar-se-lhe de sede e, aos primeiros sintomas da fome, reflui à retaguarda, fugindo ante o deserto ameaçador e estéril, aquela flora agressiva abre ao sertanejo um seio carinhoso e amigo.
+(...) 
+   A natureza toda protege o sertanejo. Talha-o como Anteu, indomável. É um titã bronzeado fazendo vacilar a marcha dos exércitos.
+CUNHA, Euclides da. Os Sertões (Campanha de Canudos). 2ª ed. São Paulo: Editora Ciranda Cultural, 2018. p. 181-186.
+Texto 2
+ESTADOS DE VIOLÊNCIA 
+   A Guerra, na longa história dos homens, terá tido seus atores e suas cenas, seus heróis e seus espaços. seus personagens e seus teatros. Diversidade incrível das fardas, dos costumes, enfeites, armaduras, equipamentos. Multiplicidade dos terrenos: barro espesso ou poeira asfixiante, brejos viscosos, desfiladeiros rochosos, prados gordurentos ou panícies sombrias, colinas acidentadas, montanhas dentadas, muros grossos das cidades fortificadas, portões e fossos profundos. Sem mesmo falar das táticas de combate, da evolução técnica das armas.
+   Mas o que malgrado tudo ficaria e basearia a distinção entre guerras maiores e menores, grandes e pequenas, verdadeiras e degradadas, era essa forma pura de fois exércitos engajando forças representando entidades políticas identificáveis, afrontando-se em batalhas decisivas, terrestres ou marítimas, que os colocavam em contato com seu princípio de encerramento: vitória ou derrota. É ainda possível essa forma pura de guerra, depois que as grandes e principais potências dispõem da arma absoluta (o fogo nuclear), depois ainda que um sí possui uma superioridade arrasadora das forças clássicas de destruição, tecnologias de reconhecimento, técnicas de fundição de precisão, depois enfim que as democracias desenvolveram uma cultura de negociação, de arbitragem em que o recurso à força nua é dado como inadequado, selvagem, contraproducente? Imagina-se que no futuro ainda grandes potências mobilizem o conjunto de suas forças vivas para se medirem? 
+   Na trama visível, dilacerada das grandes guerras contemporâneas, reconhecem-se apenas a paisagem cultural da guerra, as nervuras de sua representação dominante. Não se veem mais, e tanto melhor, colunas de soldados em centenas de milhares chegando ao futuro campo de batalha, dispondo-se em ordem para a batalha decisiva. Não se espera mais com um entusiasmo ansioso a sanção das armas: duração da batalha, data de vitória ou da derrota (...) Os estados de violência fazem aparecer uma multiplicidade de figuras novas: o terrorista, o chefe de facções, o mercenário, o soldado profissional, o engenheiro de informática, o responsável da segurança etc. Não exército disciplinado, mas redes dispersas, concorrentes, profissionais da violência. Mudanças ainda no nível do teatro dos conflitos. Para a guerra: uma planície, espaços largos, às vezes colinas ou rios, em todo caso campanhas (para não levar em conta aqui guerras de cerco). E depois vem o espetáculo desolador após a batalha: os inimigos como que abraçados na morte,
+corpos juncando o solo, fardas rasgadas, manchas de sangue. Um grande silêncio depois de tantos gritos e de vaias. O novo teatro é hoje a cidade. Não a cidade fortificada, em torno da qual se entrincheira, mas a cidade viva dos transeuntes. A dos espaços públicos: mercados, garagens, terraços de café, metrôs... A das ruas que francos atiradores isolados transformam em teatro de feira para divertimentos atrozes (...)
+   Tempos e espaços, personagens e cadáveres. Aqui se trata apenas do regime de imagens de violência armada que se acha transformado. A aposta filosófica sera dizer que acontece outra coisa, e não a guerra, que se poderia chamar provisoriamente de "estado de violência", porque eles se oporiam ao que os clássicos tinham definido como "estado de guerra" e também como "estado de natureza" (...)
+   Diante da inquietante extravagância desses conflitos dificilmente identificáveis ou codificáveis nos quadros da análise estratégica clássica, ouve-se mesmo: o pior estava por vir. 
+É preciso dizer que a polemologia (estudo da guerra) não reconhece mais seus filhos: nem seus chefes responsáveis, nem seus soldados dóceis, nem seus heróis esplêndidos, nem seus mortos no campo de honra. Chega-se mesmo a se queixar. Neste ponto, contudo, a nostalgia é dificilmente suportável. Sobretutdo para lastimar guerras que às vezes nem mesmo foram vividas pessoalmente. Estas boas velhas guerras, com bons velhos inimigos, fomentadas por Estados, alegando "razões", deve-se recordar que foram também o instrumento das mais baixas ambições, das mais loucas pretensões, dos mais sórdidos cálculos? Que elas acarretaram sem falhar o sacrifício de milhões de homens que não pediam senão para viver, que elas esgotaram precocemente civilizações desenvolvidas, conduziram culturas prestigiosas ao suicídio?
+   Resta, além de um pensamento nostálgico, compreender o que causa os estados atuais de violência. Então, antes que falar da "nova guerra", de "guerra selvagem", "guerra sem a
+guerra", de "guerra sem fim", de "guerra assimétrica", de "guerra civil generalizada", de "guerra ruiva", é preciso elucidar, em lugar do jogo antigo da guerra e da paz, as estruturações destes estados de violência (...) Como a filosofia clássica tinha conceituado o estado de guerra e de natureza, seria preciso esboçar a análise filosófica dos estados de violência, como distrubuição contemporânea das forças de destruição. 
+GROS, Frédéric. Estados de violência: ensaio sobre o fim da guerra. Tradução de José Augusto da Silva. Aparecida, SP. Editora Ideias &amp; Letras, 2009. p. 227-232 (texto adaptado).</t>
   </si>
 </sst>
 </file>
@@ -5843,7 +5841,7 @@
   <dimension ref="A1:L1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K374" sqref="K374"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -14193,7 +14191,7 @@
         <v>114</v>
       </c>
       <c r="J263" s="6" t="s">
-        <v>452</v>
+        <v>856</v>
       </c>
       <c r="K263" s="6"/>
       <c r="L263" s="6"/>
@@ -14212,10 +14210,10 @@
         <v>17</v>
       </c>
       <c r="E264" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="F264" s="3" t="s">
         <v>453</v>
-      </c>
-      <c r="F264" s="3" t="s">
-        <v>454</v>
       </c>
       <c r="G264" s="3" t="s">
         <v>32</v>
@@ -14244,7 +14242,7 @@
         <v>18</v>
       </c>
       <c r="E265" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="F265" s="5" t="s">
         <v>427</v>
@@ -14276,10 +14274,10 @@
         <v>19</v>
       </c>
       <c r="E266" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="F266" s="3" t="s">
         <v>456</v>
-      </c>
-      <c r="F266" s="3" t="s">
-        <v>457</v>
       </c>
       <c r="G266" s="3" t="s">
         <v>32</v>
@@ -14308,10 +14306,10 @@
         <v>20</v>
       </c>
       <c r="E267" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="F267" s="5" t="s">
         <v>458</v>
-      </c>
-      <c r="F267" s="5" t="s">
-        <v>459</v>
       </c>
       <c r="G267" s="5" t="s">
         <v>32</v>
@@ -14340,10 +14338,10 @@
         <v>16</v>
       </c>
       <c r="E268" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="F268" s="3" t="s">
         <v>460</v>
-      </c>
-      <c r="F268" s="3" t="s">
-        <v>461</v>
       </c>
       <c r="G268" s="3" t="s">
         <v>15</v>
@@ -14372,10 +14370,10 @@
         <v>17</v>
       </c>
       <c r="E269" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="F269" s="5" t="s">
         <v>462</v>
-      </c>
-      <c r="F269" s="5" t="s">
-        <v>463</v>
       </c>
       <c r="G269" s="5" t="s">
         <v>22</v>
@@ -14404,10 +14402,10 @@
         <v>18</v>
       </c>
       <c r="E270" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="F270" s="3" t="s">
         <v>464</v>
-      </c>
-      <c r="F270" s="3" t="s">
-        <v>465</v>
       </c>
       <c r="G270" s="3" t="s">
         <v>37</v>
@@ -14436,10 +14434,10 @@
         <v>19</v>
       </c>
       <c r="E271" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="F271" s="5" t="s">
         <v>466</v>
-      </c>
-      <c r="F271" s="5" t="s">
-        <v>467</v>
       </c>
       <c r="G271" s="5" t="s">
         <v>22</v>
@@ -14452,10 +14450,10 @@
       </c>
       <c r="J271" s="6"/>
       <c r="K271" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="L271" s="9" t="s">
         <v>468</v>
-      </c>
-      <c r="L271" s="9" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="272" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
@@ -14472,10 +14470,10 @@
         <v>20</v>
       </c>
       <c r="E272" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="F272" s="3" t="s">
         <v>470</v>
-      </c>
-      <c r="F272" s="3" t="s">
-        <v>471</v>
       </c>
       <c r="G272" s="3" t="s">
         <v>22</v>
@@ -14504,10 +14502,10 @@
         <v>21</v>
       </c>
       <c r="E273" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="F273" s="5" t="s">
         <v>472</v>
-      </c>
-      <c r="F273" s="5" t="s">
-        <v>473</v>
       </c>
       <c r="G273" s="5" t="s">
         <v>25</v>
@@ -14536,10 +14534,10 @@
         <v>22</v>
       </c>
       <c r="E274" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="F274" s="3" t="s">
         <v>474</v>
-      </c>
-      <c r="F274" s="3" t="s">
-        <v>475</v>
       </c>
       <c r="G274" s="3" t="s">
         <v>25</v>
@@ -14568,10 +14566,10 @@
         <v>23</v>
       </c>
       <c r="E275" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="F275" s="5" t="s">
         <v>476</v>
-      </c>
-      <c r="F275" s="5" t="s">
-        <v>477</v>
       </c>
       <c r="G275" s="5" t="s">
         <v>25</v>
@@ -14628,10 +14626,10 @@
         <v>25</v>
       </c>
       <c r="E277" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="F277" s="5" t="s">
         <v>478</v>
-      </c>
-      <c r="F277" s="5" t="s">
-        <v>479</v>
       </c>
       <c r="G277" s="5" t="s">
         <v>15</v>
@@ -14660,10 +14658,10 @@
         <v>26</v>
       </c>
       <c r="E278" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="F278" s="3" t="s">
         <v>480</v>
-      </c>
-      <c r="F278" s="3" t="s">
-        <v>481</v>
       </c>
       <c r="G278" s="3" t="s">
         <v>37</v>
@@ -14692,10 +14690,10 @@
         <v>27</v>
       </c>
       <c r="E279" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="F279" s="5" t="s">
         <v>482</v>
-      </c>
-      <c r="F279" s="5" t="s">
-        <v>483</v>
       </c>
       <c r="G279" s="5" t="s">
         <v>32</v>
@@ -14724,10 +14722,10 @@
         <v>28</v>
       </c>
       <c r="E280" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="F280" s="3" t="s">
         <v>484</v>
-      </c>
-      <c r="F280" s="3" t="s">
-        <v>485</v>
       </c>
       <c r="G280" s="3" t="s">
         <v>32</v>
@@ -14756,10 +14754,10 @@
         <v>29</v>
       </c>
       <c r="E281" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="F281" s="5" t="s">
         <v>486</v>
-      </c>
-      <c r="F281" s="5" t="s">
-        <v>487</v>
       </c>
       <c r="G281" s="5" t="s">
         <v>15</v>
@@ -14788,10 +14786,10 @@
         <v>30</v>
       </c>
       <c r="E282" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="F282" s="3" t="s">
         <v>488</v>
-      </c>
-      <c r="F282" s="3" t="s">
-        <v>489</v>
       </c>
       <c r="G282" s="3" t="s">
         <v>22</v>
@@ -14820,10 +14818,10 @@
         <v>1</v>
       </c>
       <c r="E283" s="5" t="s">
+        <v>489</v>
+      </c>
+      <c r="F283" s="5" t="s">
         <v>490</v>
-      </c>
-      <c r="F283" s="5" t="s">
-        <v>491</v>
       </c>
       <c r="G283" s="5" t="s">
         <v>22</v>
@@ -14835,7 +14833,7 @@
         <v>17</v>
       </c>
       <c r="J283" s="6" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="K283" s="6"/>
       <c r="L283" s="6"/>
@@ -14854,10 +14852,10 @@
         <v>2</v>
       </c>
       <c r="E284" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="F284" s="3" t="s">
         <v>493</v>
-      </c>
-      <c r="F284" s="3" t="s">
-        <v>494</v>
       </c>
       <c r="G284" s="3" t="s">
         <v>22</v>
@@ -14886,10 +14884,10 @@
         <v>3</v>
       </c>
       <c r="E285" s="5" t="s">
+        <v>494</v>
+      </c>
+      <c r="F285" s="5" t="s">
         <v>495</v>
-      </c>
-      <c r="F285" s="5" t="s">
-        <v>496</v>
       </c>
       <c r="G285" s="5" t="s">
         <v>32</v>
@@ -14918,10 +14916,10 @@
         <v>4</v>
       </c>
       <c r="E286" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="F286" s="3" t="s">
         <v>497</v>
-      </c>
-      <c r="F286" s="3" t="s">
-        <v>498</v>
       </c>
       <c r="G286" s="3" t="s">
         <v>25</v>
@@ -14950,10 +14948,10 @@
         <v>5</v>
       </c>
       <c r="E287" s="5" t="s">
+        <v>498</v>
+      </c>
+      <c r="F287" s="5" t="s">
         <v>499</v>
-      </c>
-      <c r="F287" s="5" t="s">
-        <v>500</v>
       </c>
       <c r="G287" s="5" t="s">
         <v>15</v>
@@ -14966,10 +14964,10 @@
       </c>
       <c r="J287" s="6"/>
       <c r="K287" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="L287" s="9" t="s">
         <v>501</v>
-      </c>
-      <c r="L287" s="9" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="288" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
@@ -14986,10 +14984,10 @@
         <v>6</v>
       </c>
       <c r="E288" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="F288" s="3" t="s">
         <v>503</v>
-      </c>
-      <c r="F288" s="3" t="s">
-        <v>504</v>
       </c>
       <c r="G288" s="3" t="s">
         <v>15</v>
@@ -15001,7 +14999,7 @@
         <v>17</v>
       </c>
       <c r="J288" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="K288" s="4"/>
       <c r="L288" s="4"/>
@@ -15020,10 +15018,10 @@
         <v>7</v>
       </c>
       <c r="E289" s="5" t="s">
+        <v>505</v>
+      </c>
+      <c r="F289" s="5" t="s">
         <v>506</v>
-      </c>
-      <c r="F289" s="5" t="s">
-        <v>507</v>
       </c>
       <c r="G289" s="5" t="s">
         <v>37</v>
@@ -15052,10 +15050,10 @@
         <v>8</v>
       </c>
       <c r="E290" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="F290" s="3" t="s">
         <v>508</v>
-      </c>
-      <c r="F290" s="3" t="s">
-        <v>509</v>
       </c>
       <c r="G290" s="3" t="s">
         <v>25</v>
@@ -15084,10 +15082,10 @@
         <v>9</v>
       </c>
       <c r="E291" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="F291" s="5" t="s">
         <v>510</v>
-      </c>
-      <c r="F291" s="5" t="s">
-        <v>511</v>
       </c>
       <c r="G291" s="5" t="s">
         <v>37</v>
@@ -15099,7 +15097,7 @@
         <v>17</v>
       </c>
       <c r="J291" s="6" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="K291" s="6"/>
       <c r="L291" s="6"/>
@@ -15118,10 +15116,10 @@
         <v>10</v>
       </c>
       <c r="E292" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="F292" s="3" t="s">
         <v>512</v>
-      </c>
-      <c r="F292" s="3" t="s">
-        <v>513</v>
       </c>
       <c r="G292" s="3" t="s">
         <v>32</v>
@@ -15150,10 +15148,10 @@
         <v>11</v>
       </c>
       <c r="E293" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="F293" s="5" t="s">
         <v>514</v>
-      </c>
-      <c r="F293" s="5" t="s">
-        <v>515</v>
       </c>
       <c r="G293" s="5" t="s">
         <v>37</v>
@@ -15182,10 +15180,10 @@
         <v>12</v>
       </c>
       <c r="E294" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="F294" s="3" t="s">
         <v>516</v>
-      </c>
-      <c r="F294" s="3" t="s">
-        <v>517</v>
       </c>
       <c r="G294" s="3" t="s">
         <v>37</v>
@@ -15214,10 +15212,10 @@
         <v>13</v>
       </c>
       <c r="E295" s="5" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F295" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G295" s="5" t="s">
         <v>37</v>
@@ -15246,10 +15244,10 @@
         <v>14</v>
       </c>
       <c r="E296" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="F296" s="3" t="s">
         <v>519</v>
-      </c>
-      <c r="F296" s="3" t="s">
-        <v>520</v>
       </c>
       <c r="G296" s="3" t="s">
         <v>25</v>
@@ -15278,10 +15276,10 @@
         <v>15</v>
       </c>
       <c r="E297" s="5" t="s">
+        <v>520</v>
+      </c>
+      <c r="F297" s="5" t="s">
         <v>521</v>
-      </c>
-      <c r="F297" s="5" t="s">
-        <v>522</v>
       </c>
       <c r="G297" s="5" t="s">
         <v>25</v>
@@ -15293,7 +15291,7 @@
         <v>17</v>
       </c>
       <c r="J297" s="6" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="K297" s="6"/>
       <c r="L297" s="6"/>
@@ -15312,10 +15310,10 @@
         <v>16</v>
       </c>
       <c r="E298" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="F298" s="3" t="s">
         <v>524</v>
-      </c>
-      <c r="F298" s="3" t="s">
-        <v>525</v>
       </c>
       <c r="G298" s="3" t="s">
         <v>25</v>
@@ -15344,10 +15342,10 @@
         <v>17</v>
       </c>
       <c r="E299" s="5" t="s">
+        <v>525</v>
+      </c>
+      <c r="F299" s="5" t="s">
         <v>526</v>
-      </c>
-      <c r="F299" s="5" t="s">
-        <v>527</v>
       </c>
       <c r="G299" s="5" t="s">
         <v>22</v>
@@ -15359,7 +15357,7 @@
         <v>17</v>
       </c>
       <c r="J299" s="6" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="K299" s="6"/>
       <c r="L299" s="6"/>
@@ -15378,10 +15376,10 @@
         <v>18</v>
       </c>
       <c r="E300" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="F300" s="3" t="s">
         <v>528</v>
-      </c>
-      <c r="F300" s="3" t="s">
-        <v>529</v>
       </c>
       <c r="G300" s="3" t="s">
         <v>32</v>
@@ -15410,10 +15408,10 @@
         <v>19</v>
       </c>
       <c r="E301" s="5" t="s">
+        <v>529</v>
+      </c>
+      <c r="F301" s="5" t="s">
         <v>530</v>
-      </c>
-      <c r="F301" s="5" t="s">
-        <v>531</v>
       </c>
       <c r="G301" s="5" t="s">
         <v>25</v>
@@ -15442,10 +15440,10 @@
         <v>20</v>
       </c>
       <c r="E302" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="F302" s="3" t="s">
         <v>532</v>
-      </c>
-      <c r="F302" s="3" t="s">
-        <v>533</v>
       </c>
       <c r="G302" s="3" t="s">
         <v>22</v>
@@ -15457,7 +15455,7 @@
         <v>17</v>
       </c>
       <c r="J302" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="K302" s="4"/>
       <c r="L302" s="4"/>
@@ -15476,10 +15474,10 @@
         <v>16</v>
       </c>
       <c r="E303" s="5" t="s">
+        <v>534</v>
+      </c>
+      <c r="F303" s="5" t="s">
         <v>535</v>
-      </c>
-      <c r="F303" s="5" t="s">
-        <v>536</v>
       </c>
       <c r="G303" s="5" t="s">
         <v>32</v>
@@ -15508,10 +15506,10 @@
         <v>17</v>
       </c>
       <c r="E304" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="F304" s="3" t="s">
         <v>537</v>
-      </c>
-      <c r="F304" s="3" t="s">
-        <v>538</v>
       </c>
       <c r="G304" s="3" t="s">
         <v>25</v>
@@ -15540,10 +15538,10 @@
         <v>18</v>
       </c>
       <c r="E305" s="5" t="s">
+        <v>538</v>
+      </c>
+      <c r="F305" s="5" t="s">
         <v>539</v>
-      </c>
-      <c r="F305" s="5" t="s">
-        <v>540</v>
       </c>
       <c r="G305" s="5" t="s">
         <v>32</v>
@@ -15572,10 +15570,10 @@
         <v>19</v>
       </c>
       <c r="E306" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="F306" s="3" t="s">
         <v>541</v>
-      </c>
-      <c r="F306" s="3" t="s">
-        <v>542</v>
       </c>
       <c r="G306" s="3" t="s">
         <v>15</v>
@@ -15604,10 +15602,10 @@
         <v>20</v>
       </c>
       <c r="E307" s="5" t="s">
+        <v>542</v>
+      </c>
+      <c r="F307" s="5" t="s">
         <v>543</v>
-      </c>
-      <c r="F307" s="5" t="s">
-        <v>544</v>
       </c>
       <c r="G307" s="5" t="s">
         <v>22</v>
@@ -15636,10 +15634,10 @@
         <v>21</v>
       </c>
       <c r="E308" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="F308" s="3" t="s">
         <v>545</v>
-      </c>
-      <c r="F308" s="3" t="s">
-        <v>546</v>
       </c>
       <c r="G308" s="3" t="s">
         <v>15</v>
@@ -15668,10 +15666,10 @@
         <v>22</v>
       </c>
       <c r="E309" s="5" t="s">
+        <v>546</v>
+      </c>
+      <c r="F309" s="5" t="s">
         <v>547</v>
-      </c>
-      <c r="F309" s="5" t="s">
-        <v>548</v>
       </c>
       <c r="G309" s="5" t="s">
         <v>37</v>
@@ -15700,10 +15698,10 @@
         <v>23</v>
       </c>
       <c r="E310" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="F310" s="3" t="s">
         <v>549</v>
-      </c>
-      <c r="F310" s="3" t="s">
-        <v>550</v>
       </c>
       <c r="G310" s="3" t="s">
         <v>22</v>
@@ -15732,10 +15730,10 @@
         <v>24</v>
       </c>
       <c r="E311" s="5" t="s">
+        <v>550</v>
+      </c>
+      <c r="F311" s="5" t="s">
         <v>551</v>
-      </c>
-      <c r="F311" s="5" t="s">
-        <v>552</v>
       </c>
       <c r="G311" s="5" t="s">
         <v>32</v>
@@ -15747,7 +15745,7 @@
         <v>17</v>
       </c>
       <c r="J311" s="6" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="K311" s="6"/>
       <c r="L311" s="6"/>
@@ -15766,10 +15764,10 @@
         <v>25</v>
       </c>
       <c r="E312" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="F312" s="3" t="s">
         <v>554</v>
-      </c>
-      <c r="F312" s="3" t="s">
-        <v>555</v>
       </c>
       <c r="G312" s="3" t="s">
         <v>37</v>
@@ -15782,10 +15780,10 @@
       </c>
       <c r="J312" s="4"/>
       <c r="K312" s="4" t="s">
+        <v>555</v>
+      </c>
+      <c r="L312" s="7" t="s">
         <v>556</v>
-      </c>
-      <c r="L312" s="7" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="313" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
@@ -15802,10 +15800,10 @@
         <v>26</v>
       </c>
       <c r="E313" s="5" t="s">
+        <v>557</v>
+      </c>
+      <c r="F313" s="5" t="s">
         <v>558</v>
-      </c>
-      <c r="F313" s="5" t="s">
-        <v>559</v>
       </c>
       <c r="G313" s="5" t="s">
         <v>15</v>
@@ -15834,10 +15832,10 @@
         <v>27</v>
       </c>
       <c r="E314" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="F314" s="3" t="s">
         <v>560</v>
-      </c>
-      <c r="F314" s="3" t="s">
-        <v>561</v>
       </c>
       <c r="G314" s="3" t="s">
         <v>25</v>
@@ -15866,10 +15864,10 @@
         <v>28</v>
       </c>
       <c r="E315" s="5" t="s">
+        <v>561</v>
+      </c>
+      <c r="F315" s="5" t="s">
         <v>562</v>
-      </c>
-      <c r="F315" s="5" t="s">
-        <v>563</v>
       </c>
       <c r="G315" s="5" t="s">
         <v>15</v>
@@ -15898,10 +15896,10 @@
         <v>29</v>
       </c>
       <c r="E316" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="F316" s="3" t="s">
         <v>564</v>
-      </c>
-      <c r="F316" s="3" t="s">
-        <v>565</v>
       </c>
       <c r="G316" s="3" t="s">
         <v>32</v>
@@ -15930,10 +15928,10 @@
         <v>30</v>
       </c>
       <c r="E317" s="5" t="s">
+        <v>565</v>
+      </c>
+      <c r="F317" s="5" t="s">
         <v>566</v>
-      </c>
-      <c r="F317" s="5" t="s">
-        <v>567</v>
       </c>
       <c r="G317" s="5" t="s">
         <v>25</v>
@@ -15962,10 +15960,10 @@
         <v>1</v>
       </c>
       <c r="E318" s="3" t="s">
+        <v>567</v>
+      </c>
+      <c r="F318" s="3" t="s">
         <v>568</v>
-      </c>
-      <c r="F318" s="3" t="s">
-        <v>569</v>
       </c>
       <c r="G318" s="3" t="s">
         <v>22</v>
@@ -15977,7 +15975,7 @@
         <v>17</v>
       </c>
       <c r="J318" s="4" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="K318" s="4"/>
       <c r="L318" s="7"/>
@@ -15996,10 +15994,10 @@
         <v>2</v>
       </c>
       <c r="E319" s="5" t="s">
+        <v>570</v>
+      </c>
+      <c r="F319" s="5" t="s">
         <v>571</v>
-      </c>
-      <c r="F319" s="5" t="s">
-        <v>572</v>
       </c>
       <c r="G319" s="5" t="s">
         <v>15</v>
@@ -16028,10 +16026,10 @@
         <v>3</v>
       </c>
       <c r="E320" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="F320" s="3" t="s">
         <v>573</v>
-      </c>
-      <c r="F320" s="3" t="s">
-        <v>574</v>
       </c>
       <c r="G320" s="3" t="s">
         <v>32</v>
@@ -16043,7 +16041,7 @@
         <v>17</v>
       </c>
       <c r="J320" s="4" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="K320" s="4"/>
       <c r="L320" s="4"/>
@@ -16062,10 +16060,10 @@
         <v>4</v>
       </c>
       <c r="E321" s="5" t="s">
+        <v>574</v>
+      </c>
+      <c r="F321" s="5" t="s">
         <v>575</v>
-      </c>
-      <c r="F321" s="5" t="s">
-        <v>576</v>
       </c>
       <c r="G321" s="5" t="s">
         <v>25</v>
@@ -16094,10 +16092,10 @@
         <v>5</v>
       </c>
       <c r="E322" s="3" t="s">
+        <v>576</v>
+      </c>
+      <c r="F322" s="3" t="s">
         <v>577</v>
-      </c>
-      <c r="F322" s="3" t="s">
-        <v>578</v>
       </c>
       <c r="G322" s="3" t="s">
         <v>37</v>
@@ -16126,10 +16124,10 @@
         <v>6</v>
       </c>
       <c r="E323" s="5" t="s">
+        <v>578</v>
+      </c>
+      <c r="F323" s="5" t="s">
         <v>579</v>
-      </c>
-      <c r="F323" s="5" t="s">
-        <v>580</v>
       </c>
       <c r="G323" s="5" t="s">
         <v>15</v>
@@ -16158,10 +16156,10 @@
         <v>7</v>
       </c>
       <c r="E324" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="F324" s="3" t="s">
         <v>581</v>
-      </c>
-      <c r="F324" s="3" t="s">
-        <v>582</v>
       </c>
       <c r="G324" s="3" t="s">
         <v>37</v>
@@ -16190,10 +16188,10 @@
         <v>8</v>
       </c>
       <c r="E325" s="5" t="s">
+        <v>582</v>
+      </c>
+      <c r="F325" s="5" t="s">
         <v>583</v>
-      </c>
-      <c r="F325" s="5" t="s">
-        <v>584</v>
       </c>
       <c r="G325" s="5" t="s">
         <v>32</v>
@@ -16222,10 +16220,10 @@
         <v>9</v>
       </c>
       <c r="E326" s="3" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="F326" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="G326" s="3" t="s">
         <v>22</v>
@@ -16254,10 +16252,10 @@
         <v>10</v>
       </c>
       <c r="E327" s="5" t="s">
+        <v>585</v>
+      </c>
+      <c r="F327" s="5" t="s">
         <v>586</v>
-      </c>
-      <c r="F327" s="5" t="s">
-        <v>587</v>
       </c>
       <c r="G327" s="5" t="s">
         <v>37</v>
@@ -16286,10 +16284,10 @@
         <v>11</v>
       </c>
       <c r="E328" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="F328" s="3" t="s">
         <v>588</v>
-      </c>
-      <c r="F328" s="3" t="s">
-        <v>589</v>
       </c>
       <c r="G328" s="3" t="s">
         <v>25</v>
@@ -16318,10 +16316,10 @@
         <v>12</v>
       </c>
       <c r="E329" s="5" t="s">
+        <v>589</v>
+      </c>
+      <c r="F329" s="5" t="s">
         <v>590</v>
-      </c>
-      <c r="F329" s="5" t="s">
-        <v>591</v>
       </c>
       <c r="G329" s="5" t="s">
         <v>32</v>
@@ -16350,10 +16348,10 @@
         <v>13</v>
       </c>
       <c r="E330" s="3" t="s">
+        <v>591</v>
+      </c>
+      <c r="F330" s="3" t="s">
         <v>592</v>
-      </c>
-      <c r="F330" s="3" t="s">
-        <v>593</v>
       </c>
       <c r="G330" s="3" t="s">
         <v>32</v>
@@ -16382,10 +16380,10 @@
         <v>14</v>
       </c>
       <c r="E331" s="5" t="s">
+        <v>593</v>
+      </c>
+      <c r="F331" s="5" t="s">
         <v>594</v>
-      </c>
-      <c r="F331" s="5" t="s">
-        <v>595</v>
       </c>
       <c r="G331" s="5" t="s">
         <v>37</v>
@@ -16414,10 +16412,10 @@
         <v>15</v>
       </c>
       <c r="E332" s="12" t="s">
+        <v>595</v>
+      </c>
+      <c r="F332" s="3" t="s">
         <v>596</v>
-      </c>
-      <c r="F332" s="3" t="s">
-        <v>597</v>
       </c>
       <c r="G332" s="3" t="s">
         <v>22</v>
@@ -16430,10 +16428,10 @@
       </c>
       <c r="J332" s="4"/>
       <c r="K332" s="4" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="L332" s="4" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
     </row>
     <row r="333" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
@@ -16450,10 +16448,10 @@
         <v>16</v>
       </c>
       <c r="E333" s="5" t="s">
+        <v>597</v>
+      </c>
+      <c r="F333" s="5" t="s">
         <v>598</v>
-      </c>
-      <c r="F333" s="5" t="s">
-        <v>599</v>
       </c>
       <c r="G333" s="5" t="s">
         <v>22</v>
@@ -16465,7 +16463,7 @@
         <v>114</v>
       </c>
       <c r="J333" s="6" t="s">
-        <v>600</v>
+        <v>857</v>
       </c>
       <c r="K333" s="6"/>
       <c r="L333" s="6"/>
@@ -16484,10 +16482,10 @@
         <v>17</v>
       </c>
       <c r="E334" s="3" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="F334" s="3" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="G334" s="3" t="s">
         <v>25</v>
@@ -16499,7 +16497,7 @@
         <v>114</v>
       </c>
       <c r="J334" s="4" t="s">
-        <v>600</v>
+        <v>857</v>
       </c>
       <c r="K334" s="4"/>
       <c r="L334" s="4"/>
@@ -16518,10 +16516,10 @@
         <v>18</v>
       </c>
       <c r="E335" s="5" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="F335" s="5" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="G335" s="5" t="s">
         <v>15</v>
@@ -16550,10 +16548,10 @@
         <v>19</v>
       </c>
       <c r="E336" s="3" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="F336" s="3" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="G336" s="3" t="s">
         <v>25</v>
@@ -16582,10 +16580,10 @@
         <v>20</v>
       </c>
       <c r="E337" s="5" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="F337" s="5" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="G337" s="5" t="s">
         <v>15</v>
@@ -16614,10 +16612,10 @@
         <v>16</v>
       </c>
       <c r="E338" s="3" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="F338" s="3" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="G338" s="3" t="s">
         <v>15</v>
@@ -16646,10 +16644,10 @@
         <v>17</v>
       </c>
       <c r="E339" s="5" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="F339" s="5" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="G339" s="5" t="s">
         <v>25</v>
@@ -16678,10 +16676,10 @@
         <v>18</v>
       </c>
       <c r="E340" s="3" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="F340" s="3" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="G340" s="3" t="s">
         <v>25</v>
@@ -16710,10 +16708,10 @@
         <v>19</v>
       </c>
       <c r="E341" s="5" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="F341" s="5" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="G341" s="5" t="s">
         <v>32</v>
@@ -16742,10 +16740,10 @@
         <v>20</v>
       </c>
       <c r="E342" s="3" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="F342" s="3" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="G342" s="3" t="s">
         <v>37</v>
@@ -16774,10 +16772,10 @@
         <v>21</v>
       </c>
       <c r="E343" s="5" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="F343" s="5" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="G343" s="5" t="s">
         <v>25</v>
@@ -16806,10 +16804,10 @@
         <v>22</v>
       </c>
       <c r="E344" s="3" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="F344" s="3" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="G344" s="3" t="s">
         <v>22</v>
@@ -16838,10 +16836,10 @@
         <v>23</v>
       </c>
       <c r="E345" s="5" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="F345" s="5" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="G345" s="5" t="s">
         <v>32</v>
@@ -16870,10 +16868,10 @@
         <v>24</v>
       </c>
       <c r="E346" s="3" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="F346" s="3" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="G346" s="3" t="s">
         <v>37</v>
@@ -16902,10 +16900,10 @@
         <v>25</v>
       </c>
       <c r="E347" s="5" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="F347" s="5" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="G347" s="5" t="s">
         <v>32</v>
@@ -16918,10 +16916,10 @@
       </c>
       <c r="J347" s="6"/>
       <c r="K347" s="6" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="L347" s="9" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="348" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
@@ -16938,10 +16936,10 @@
         <v>26</v>
       </c>
       <c r="E348" s="3" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="F348" s="3" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="G348" s="3" t="s">
         <v>22</v>
@@ -16970,10 +16968,10 @@
         <v>27</v>
       </c>
       <c r="E349" s="5" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="F349" s="5" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="G349" s="5" t="s">
         <v>25</v>
@@ -17002,10 +17000,10 @@
         <v>28</v>
       </c>
       <c r="E350" s="3" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="F350" s="3" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="G350" s="3" t="s">
         <v>37</v>
@@ -17034,10 +17032,10 @@
         <v>29</v>
       </c>
       <c r="E351" s="5" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="F351" s="5" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="G351" s="5" t="s">
         <v>32</v>
@@ -17066,10 +17064,10 @@
         <v>30</v>
       </c>
       <c r="E352" s="3" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="F352" s="3" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="G352" s="3" t="s">
         <v>22</v>
@@ -17098,10 +17096,10 @@
         <v>1</v>
       </c>
       <c r="E353" s="5" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="F353" s="5" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="G353" s="5" t="s">
         <v>25</v>
@@ -17113,7 +17111,7 @@
         <v>17</v>
       </c>
       <c r="J353" s="6" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="K353" s="6"/>
       <c r="L353" s="6"/>
@@ -17132,10 +17130,10 @@
         <v>2</v>
       </c>
       <c r="E354" s="3" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="F354" s="3" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="G354" s="3" t="s">
         <v>37</v>
@@ -17147,7 +17145,7 @@
         <v>17</v>
       </c>
       <c r="J354" s="4" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="K354" s="4"/>
       <c r="L354" s="4"/>
@@ -17166,10 +17164,10 @@
         <v>3</v>
       </c>
       <c r="E355" s="5" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="F355" s="5" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G355" s="5" t="s">
         <v>37</v>
@@ -17181,7 +17179,7 @@
         <v>17</v>
       </c>
       <c r="J355" s="6" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="K355" s="6"/>
       <c r="L355" s="6"/>
@@ -17200,10 +17198,10 @@
         <v>4</v>
       </c>
       <c r="E356" s="3" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="F356" s="3" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="G356" s="3" t="s">
         <v>15</v>
@@ -17232,10 +17230,10 @@
         <v>5</v>
       </c>
       <c r="E357" s="5" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="F357" s="5" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="G357" s="5" t="s">
         <v>15</v>
@@ -17264,10 +17262,10 @@
         <v>6</v>
       </c>
       <c r="E358" s="3" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="F358" s="3" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="G358" s="3" t="s">
         <v>22</v>
@@ -17296,10 +17294,10 @@
         <v>7</v>
       </c>
       <c r="E359" s="5" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="F359" s="5" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="G359" s="5" t="s">
         <v>15</v>
@@ -17311,7 +17309,7 @@
         <v>17</v>
       </c>
       <c r="J359" s="6" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="K359" s="6"/>
       <c r="L359" s="6"/>
@@ -17330,10 +17328,10 @@
         <v>8</v>
       </c>
       <c r="E360" s="3" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="F360" s="3" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="G360" s="3" t="s">
         <v>22</v>
@@ -17362,10 +17360,10 @@
         <v>9</v>
       </c>
       <c r="E361" s="5" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="F361" s="5" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="G361" s="5" t="s">
         <v>22</v>
@@ -17394,10 +17392,10 @@
         <v>10</v>
       </c>
       <c r="E362" s="3" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="F362" s="3" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="G362" s="3" t="s">
         <v>37</v>
@@ -17410,10 +17408,10 @@
       </c>
       <c r="J362" s="4"/>
       <c r="K362" s="4" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="L362" s="7" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="363" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
@@ -17430,10 +17428,10 @@
         <v>11</v>
       </c>
       <c r="E363" s="5" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="F363" s="5" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="G363" s="5" t="s">
         <v>22</v>
@@ -17462,10 +17460,10 @@
         <v>12</v>
       </c>
       <c r="E364" s="3" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="F364" s="3" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="G364" s="3" t="s">
         <v>15</v>
@@ -17494,10 +17492,10 @@
         <v>13</v>
       </c>
       <c r="E365" s="5" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="F365" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="G365" s="5" t="s">
         <v>25</v>
@@ -17526,10 +17524,10 @@
         <v>14</v>
       </c>
       <c r="E366" s="3" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="F366" s="3" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="G366" s="3" t="s">
         <v>32</v>
@@ -17558,10 +17556,10 @@
         <v>15</v>
       </c>
       <c r="E367" s="5" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="F367" s="5" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="G367" s="5" t="s">
         <v>32</v>
@@ -17590,10 +17588,10 @@
         <v>16</v>
       </c>
       <c r="E368" s="3" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="F368" s="3" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="G368" s="3" t="s">
         <v>25</v>
@@ -17622,10 +17620,10 @@
         <v>17</v>
       </c>
       <c r="E369" s="5" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="F369" s="5" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="G369" s="5" t="s">
         <v>22</v>
@@ -17637,7 +17635,7 @@
         <v>17</v>
       </c>
       <c r="J369" s="6" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="K369" s="6"/>
       <c r="L369" s="6"/>
@@ -17656,10 +17654,10 @@
         <v>18</v>
       </c>
       <c r="E370" s="3" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="F370" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="G370" s="3" t="s">
         <v>22</v>
@@ -17688,10 +17686,10 @@
         <v>19</v>
       </c>
       <c r="E371" s="5" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="F371" s="5" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="G371" s="5" t="s">
         <v>32</v>
@@ -17703,7 +17701,7 @@
         <v>17</v>
       </c>
       <c r="J371" s="6" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="K371" s="6"/>
       <c r="L371" s="6"/>
@@ -17722,10 +17720,10 @@
         <v>20</v>
       </c>
       <c r="E372" s="3" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="F372" s="3" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="G372" s="3" t="s">
         <v>25</v>
@@ -17737,7 +17735,7 @@
         <v>17</v>
       </c>
       <c r="J372" s="4" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="K372" s="4"/>
       <c r="L372" s="4"/>
@@ -17756,16 +17754,16 @@
         <v>49</v>
       </c>
       <c r="E373" s="5" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="F373" s="5" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="G373" s="5" t="s">
         <v>22</v>
       </c>
       <c r="H373" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I373" s="6" t="s">
         <v>17</v>
@@ -17788,28 +17786,28 @@
         <v>50</v>
       </c>
       <c r="E374" s="3" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="F374" s="3" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="G374" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H374" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I374" s="4" t="s">
         <v>17</v>
       </c>
       <c r="J374" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="K374" s="4" t="s">
+        <v>690</v>
+      </c>
+      <c r="L374" s="7" t="s">
         <v>691</v>
-      </c>
-      <c r="K374" s="4" t="s">
-        <v>692</v>
-      </c>
-      <c r="L374" s="7" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="375" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
@@ -17826,16 +17824,16 @@
         <v>51</v>
       </c>
       <c r="E375" s="5" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="F375" s="5" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="G375" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H375" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I375" s="6" t="s">
         <v>17</v>
@@ -17863,7 +17861,7 @@
         <v>32</v>
       </c>
       <c r="H376" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I376" s="4" t="s">
         <v>114</v>
@@ -17893,7 +17891,7 @@
         <v>32</v>
       </c>
       <c r="H377" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I377" s="6" t="s">
         <v>114</v>
@@ -17918,16 +17916,16 @@
         <v>54</v>
       </c>
       <c r="E378" s="3" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="F378" s="3" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="G378" s="3" t="s">
         <v>37</v>
       </c>
       <c r="H378" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I378" s="4" t="s">
         <v>17</v>
@@ -17950,16 +17948,16 @@
         <v>55</v>
       </c>
       <c r="E379" s="5" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="F379" s="5" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="G379" s="5" t="s">
         <v>37</v>
       </c>
       <c r="H379" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I379" s="6" t="s">
         <v>17</v>
@@ -17982,16 +17980,16 @@
         <v>56</v>
       </c>
       <c r="E380" s="3" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="F380" s="3" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="G380" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H380" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I380" s="4" t="s">
         <v>17</v>
@@ -18014,16 +18012,16 @@
         <v>57</v>
       </c>
       <c r="E381" s="5" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="F381" s="5" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="G381" s="5" t="s">
         <v>22</v>
       </c>
       <c r="H381" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I381" s="6" t="s">
         <v>17</v>
@@ -18046,16 +18044,16 @@
         <v>58</v>
       </c>
       <c r="E382" s="3" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="F382" s="3" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="G382" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H382" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I382" s="4" t="s">
         <v>17</v>
@@ -18078,16 +18076,16 @@
         <v>59</v>
       </c>
       <c r="E383" s="5" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="F383" s="5" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="G383" s="5" t="s">
         <v>37</v>
       </c>
       <c r="H383" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I383" s="6" t="s">
         <v>17</v>
@@ -18115,7 +18113,7 @@
         <v>25</v>
       </c>
       <c r="H384" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I384" s="4" t="s">
         <v>114</v>
@@ -18140,16 +18138,16 @@
         <v>31</v>
       </c>
       <c r="E385" s="5" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="F385" s="5" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="G385" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H385" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I385" s="6" t="s">
         <v>17</v>
@@ -18172,16 +18170,16 @@
         <v>32</v>
       </c>
       <c r="E386" s="3" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="F386" s="3" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="G386" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H386" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I386" s="4" t="s">
         <v>17</v>
@@ -18204,16 +18202,16 @@
         <v>33</v>
       </c>
       <c r="E387" s="5" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="F387" s="5" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="G387" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H387" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I387" s="6" t="s">
         <v>17</v>
@@ -18241,13 +18239,13 @@
         <v>22</v>
       </c>
       <c r="H388" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I388" s="4" t="s">
         <v>114</v>
       </c>
       <c r="J388" s="4" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="K388" s="4"/>
       <c r="L388" s="4"/>
@@ -18266,26 +18264,26 @@
         <v>35</v>
       </c>
       <c r="E389" s="5" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="F389" s="5" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="G389" s="5" t="s">
         <v>22</v>
       </c>
       <c r="H389" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I389" s="6" t="s">
         <v>17</v>
       </c>
       <c r="J389" s="6"/>
       <c r="K389" s="6" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="L389" s="9" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
     </row>
     <row r="390" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
@@ -18307,7 +18305,7 @@
         <v>15</v>
       </c>
       <c r="H390" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I390" s="4" t="s">
         <v>114</v>
@@ -18337,7 +18335,7 @@
         <v>25</v>
       </c>
       <c r="H391" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I391" s="6" t="s">
         <v>114</v>
@@ -18367,7 +18365,7 @@
         <v>37</v>
       </c>
       <c r="H392" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I392" s="4" t="s">
         <v>114</v>
@@ -18392,16 +18390,16 @@
         <v>39</v>
       </c>
       <c r="E393" s="5" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="F393" s="5" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="G393" s="5" t="s">
         <v>22</v>
       </c>
       <c r="H393" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I393" s="6" t="s">
         <v>17</v>
@@ -18429,7 +18427,7 @@
         <v>113</v>
       </c>
       <c r="H394" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I394" s="4" t="s">
         <v>114</v>
@@ -18452,16 +18450,16 @@
         <v>56</v>
       </c>
       <c r="E395" s="5" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="F395" s="5" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="G395" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H395" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I395" s="6" t="s">
         <v>17</v>
@@ -18484,16 +18482,16 @@
         <v>57</v>
       </c>
       <c r="E396" s="3" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="F396" s="3" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="G396" s="3" t="s">
         <v>32</v>
       </c>
       <c r="H396" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I396" s="4" t="s">
         <v>17</v>
@@ -18516,26 +18514,26 @@
         <v>58</v>
       </c>
       <c r="E397" s="5" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="F397" s="5" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="G397" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H397" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I397" s="6" t="s">
         <v>17</v>
       </c>
       <c r="J397" s="6"/>
       <c r="K397" s="6" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="L397" s="9" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="398" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
@@ -18552,16 +18550,16 @@
         <v>59</v>
       </c>
       <c r="E398" s="3" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="F398" s="3" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="G398" s="3" t="s">
         <v>37</v>
       </c>
       <c r="H398" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I398" s="4" t="s">
         <v>17</v>
@@ -18589,7 +18587,7 @@
         <v>113</v>
       </c>
       <c r="H399" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I399" s="6" t="s">
         <v>114</v>
@@ -18612,16 +18610,16 @@
         <v>61</v>
       </c>
       <c r="E400" s="3" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="F400" s="3" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="G400" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H400" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I400" s="4" t="s">
         <v>17</v>
@@ -18649,7 +18647,7 @@
         <v>32</v>
       </c>
       <c r="H401" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I401" s="6" t="s">
         <v>114</v>
@@ -18674,16 +18672,16 @@
         <v>63</v>
       </c>
       <c r="E402" s="3" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="F402" s="3" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="G402" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H402" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I402" s="4" t="s">
         <v>17</v>
@@ -18706,16 +18704,16 @@
         <v>64</v>
       </c>
       <c r="E403" s="5" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="F403" s="5" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="G403" s="5" t="s">
         <v>37</v>
       </c>
       <c r="H403" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I403" s="6" t="s">
         <v>17</v>
@@ -18738,16 +18736,16 @@
         <v>65</v>
       </c>
       <c r="E404" s="3" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="F404" s="3" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="G404" s="3" t="s">
         <v>32</v>
       </c>
       <c r="H404" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I404" s="4" t="s">
         <v>17</v>
@@ -18770,16 +18768,16 @@
         <v>66</v>
       </c>
       <c r="E405" s="5" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="F405" s="5" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="G405" s="5" t="s">
         <v>22</v>
       </c>
       <c r="H405" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I405" s="6" t="s">
         <v>17</v>
@@ -18802,16 +18800,16 @@
         <v>67</v>
       </c>
       <c r="E406" s="3" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="F406" s="3" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="G406" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H406" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I406" s="4" t="s">
         <v>17</v>
@@ -18834,16 +18832,16 @@
         <v>68</v>
       </c>
       <c r="E407" s="5" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="F407" s="5" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="G407" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H407" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I407" s="6" t="s">
         <v>17</v>
@@ -18871,7 +18869,7 @@
         <v>22</v>
       </c>
       <c r="H408" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I408" s="4" t="s">
         <v>114</v>
@@ -18896,16 +18894,16 @@
         <v>70</v>
       </c>
       <c r="E409" s="5" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="F409" s="5" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="G409" s="5" t="s">
         <v>37</v>
       </c>
       <c r="H409" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I409" s="6" t="s">
         <v>17</v>
@@ -18928,26 +18926,26 @@
         <v>31</v>
       </c>
       <c r="E410" s="3" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="F410" s="3" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="G410" s="3" t="s">
         <v>32</v>
       </c>
       <c r="H410" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I410" s="4" t="s">
         <v>17</v>
       </c>
       <c r="J410" s="4"/>
       <c r="K410" s="4" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="L410" s="7" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
     </row>
     <row r="411" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
@@ -18964,16 +18962,16 @@
         <v>32</v>
       </c>
       <c r="E411" s="5" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="F411" s="5" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="G411" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H411" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I411" s="6" t="s">
         <v>17</v>
@@ -18996,16 +18994,16 @@
         <v>33</v>
       </c>
       <c r="E412" s="3" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="F412" s="3" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="G412" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H412" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I412" s="4" t="s">
         <v>17</v>
@@ -19033,7 +19031,7 @@
         <v>22</v>
       </c>
       <c r="H413" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I413" s="6" t="s">
         <v>114</v>
@@ -19058,16 +19056,16 @@
         <v>35</v>
       </c>
       <c r="E414" s="3" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="F414" s="3" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="G414" s="3" t="s">
         <v>32</v>
       </c>
       <c r="H414" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I414" s="4" t="s">
         <v>17</v>
@@ -19090,16 +19088,16 @@
         <v>36</v>
       </c>
       <c r="E415" s="5" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F415" s="5" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="G415" s="5" t="s">
         <v>15</v>
       </c>
       <c r="H415" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I415" s="6" t="s">
         <v>17</v>
@@ -19127,7 +19125,7 @@
         <v>32</v>
       </c>
       <c r="H416" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I416" s="4" t="s">
         <v>114</v>
@@ -19152,16 +19150,16 @@
         <v>38</v>
       </c>
       <c r="E417" s="5" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="F417" s="5" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="G417" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H417" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I417" s="6" t="s">
         <v>17</v>
@@ -19184,16 +19182,16 @@
         <v>39</v>
       </c>
       <c r="E418" s="3" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="F418" s="3" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="G418" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H418" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I418" s="4" t="s">
         <v>17</v>
@@ -19216,16 +19214,16 @@
         <v>40</v>
       </c>
       <c r="E419" s="5" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="F419" s="5" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="G419" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H419" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I419" s="6" t="s">
         <v>17</v>
@@ -19248,16 +19246,16 @@
         <v>56</v>
       </c>
       <c r="E420" s="3" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="F420" s="3" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="G420" s="3" t="s">
         <v>32</v>
       </c>
       <c r="H420" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I420" s="4" t="s">
         <v>17</v>
@@ -19280,22 +19278,22 @@
         <v>57</v>
       </c>
       <c r="E421" s="5" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="F421" s="5" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="G421" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H421" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I421" s="6" t="s">
         <v>17</v>
       </c>
       <c r="J421" s="6" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="K421" s="6"/>
       <c r="L421" s="6"/>
@@ -19314,16 +19312,16 @@
         <v>58</v>
       </c>
       <c r="E422" s="3" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="F422" s="3" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="G422" s="3" t="s">
         <v>32</v>
       </c>
       <c r="H422" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I422" s="4" t="s">
         <v>17</v>
@@ -19346,16 +19344,16 @@
         <v>59</v>
       </c>
       <c r="E423" s="5" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F423" s="5" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="G423" s="5" t="s">
         <v>22</v>
       </c>
       <c r="H423" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I423" s="6" t="s">
         <v>17</v>
@@ -19378,16 +19376,16 @@
         <v>60</v>
       </c>
       <c r="E424" s="3" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="F424" s="3" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="G424" s="3" t="s">
         <v>32</v>
       </c>
       <c r="H424" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I424" s="4" t="s">
         <v>17</v>
@@ -19410,16 +19408,16 @@
         <v>61</v>
       </c>
       <c r="E425" s="5" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="F425" s="5" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="G425" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H425" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I425" s="6" t="s">
         <v>17</v>
@@ -19447,7 +19445,7 @@
         <v>22</v>
       </c>
       <c r="H426" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I426" s="4" t="s">
         <v>114</v>
@@ -19472,16 +19470,16 @@
         <v>63</v>
       </c>
       <c r="E427" s="5" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="F427" s="5" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="G427" s="5" t="s">
         <v>37</v>
       </c>
       <c r="H427" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I427" s="6" t="s">
         <v>17</v>
@@ -19504,16 +19502,16 @@
         <v>64</v>
       </c>
       <c r="E428" s="3" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="F428" s="3" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="G428" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H428" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I428" s="4" t="s">
         <v>17</v>
@@ -19536,16 +19534,16 @@
         <v>65</v>
       </c>
       <c r="E429" s="5" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="F429" s="5" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="G429" s="5" t="s">
         <v>15</v>
       </c>
       <c r="H429" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I429" s="6" t="s">
         <v>17</v>
@@ -19568,16 +19566,16 @@
         <v>66</v>
       </c>
       <c r="E430" s="3" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="F430" s="3" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="G430" s="3" t="s">
         <v>37</v>
       </c>
       <c r="H430" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I430" s="4" t="s">
         <v>17</v>
@@ -19600,16 +19598,16 @@
         <v>67</v>
       </c>
       <c r="E431" s="5" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="F431" s="5" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G431" s="5" t="s">
         <v>22</v>
       </c>
       <c r="H431" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I431" s="6" t="s">
         <v>17</v>
@@ -19637,7 +19635,7 @@
         <v>22</v>
       </c>
       <c r="H432" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I432" s="4" t="s">
         <v>114</v>
@@ -19662,28 +19660,28 @@
         <v>69</v>
       </c>
       <c r="E433" s="5" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="F433" s="5" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="G433" s="5" t="s">
         <v>37</v>
       </c>
       <c r="H433" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I433" s="6" t="s">
         <v>17</v>
       </c>
       <c r="J433" s="6" t="s">
+        <v>788</v>
+      </c>
+      <c r="K433" s="6" t="s">
+        <v>789</v>
+      </c>
+      <c r="L433" s="9" t="s">
         <v>790</v>
-      </c>
-      <c r="K433" s="6" t="s">
-        <v>791</v>
-      </c>
-      <c r="L433" s="9" t="s">
-        <v>792</v>
       </c>
     </row>
     <row r="434" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
@@ -19705,7 +19703,7 @@
         <v>15</v>
       </c>
       <c r="H434" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I434" s="4" t="s">
         <v>114</v>
@@ -19730,26 +19728,26 @@
         <v>31</v>
       </c>
       <c r="E435" s="5" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="F435" s="5" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="G435" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H435" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I435" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J435" s="5"/>
       <c r="K435" s="5" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="L435" s="10" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
     </row>
     <row r="436" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
@@ -19766,16 +19764,16 @@
         <v>32</v>
       </c>
       <c r="E436" s="3" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="F436" s="3" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="G436" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H436" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I436" s="4" t="s">
         <v>17</v>
@@ -19798,16 +19796,16 @@
         <v>33</v>
       </c>
       <c r="E437" s="5" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F437" s="5" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="G437" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H437" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I437" s="6" t="s">
         <v>17</v>
@@ -19830,16 +19828,16 @@
         <v>34</v>
       </c>
       <c r="E438" s="3" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="F438" s="3" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="G438" s="3" t="s">
         <v>32</v>
       </c>
       <c r="H438" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I438" s="4" t="s">
         <v>17</v>
@@ -19862,16 +19860,16 @@
         <v>35</v>
       </c>
       <c r="E439" s="5" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="F439" s="5" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="G439" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H439" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I439" s="6" t="s">
         <v>17</v>
@@ -19894,16 +19892,16 @@
         <v>36</v>
       </c>
       <c r="E440" s="3" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="F440" s="3" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="G440" s="3" t="s">
         <v>22</v>
       </c>
       <c r="H440" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I440" s="4" t="s">
         <v>17</v>
@@ -19926,16 +19924,16 @@
         <v>37</v>
       </c>
       <c r="E441" s="5" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="F441" s="5" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="G441" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H441" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I441" s="6" t="s">
         <v>17</v>
@@ -19958,16 +19956,16 @@
         <v>38</v>
       </c>
       <c r="E442" s="3" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="F442" s="3" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="G442" s="3" t="s">
         <v>22</v>
       </c>
       <c r="H442" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I442" s="4" t="s">
         <v>17</v>
@@ -19990,16 +19988,16 @@
         <v>39</v>
       </c>
       <c r="E443" s="5" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="F443" s="5" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="G443" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H443" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I443" s="6" t="s">
         <v>17</v>
@@ -20022,16 +20020,16 @@
         <v>40</v>
       </c>
       <c r="E444" s="3" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="F444" s="3" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="G444" s="3" t="s">
         <v>32</v>
       </c>
       <c r="H444" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I444" s="4" t="s">
         <v>17</v>
@@ -20054,16 +20052,16 @@
         <v>56</v>
       </c>
       <c r="E445" s="5" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="F445" s="5" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="G445" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H445" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I445" s="6" t="s">
         <v>17</v>
@@ -20086,16 +20084,16 @@
         <v>57</v>
       </c>
       <c r="E446" s="3" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="F446" s="3" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="G446" s="3" t="s">
         <v>37</v>
       </c>
       <c r="H446" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I446" s="4" t="s">
         <v>17</v>
@@ -20118,16 +20116,16 @@
         <v>58</v>
       </c>
       <c r="E447" s="5" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="F447" s="5" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="G447" s="5" t="s">
         <v>22</v>
       </c>
       <c r="H447" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I447" s="6" t="s">
         <v>17</v>
@@ -20150,16 +20148,16 @@
         <v>59</v>
       </c>
       <c r="E448" s="3" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="F448" s="3" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="G448" s="3" t="s">
         <v>32</v>
       </c>
       <c r="H448" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I448" s="4" t="s">
         <v>17</v>
@@ -20187,7 +20185,7 @@
         <v>113</v>
       </c>
       <c r="H449" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I449" s="6" t="s">
         <v>114</v>
@@ -20210,16 +20208,16 @@
         <v>61</v>
       </c>
       <c r="E450" s="3" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="F450" s="3" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="G450" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H450" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I450" s="4" t="s">
         <v>17</v>
@@ -20242,16 +20240,16 @@
         <v>62</v>
       </c>
       <c r="E451" s="5" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="F451" s="5" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="G451" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H451" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I451" s="6" t="s">
         <v>17</v>
@@ -20274,16 +20272,16 @@
         <v>63</v>
       </c>
       <c r="E452" s="3" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="F452" s="3" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="G452" s="3" t="s">
         <v>22</v>
       </c>
       <c r="H452" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I452" s="4" t="s">
         <v>17</v>
@@ -20306,26 +20304,26 @@
         <v>64</v>
       </c>
       <c r="E453" s="5" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="F453" s="5" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="G453" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H453" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I453" s="6" t="s">
         <v>17</v>
       </c>
       <c r="J453" s="6"/>
       <c r="K453" s="6" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="L453" s="9" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
     </row>
     <row r="454" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
@@ -20342,16 +20340,16 @@
         <v>65</v>
       </c>
       <c r="E454" s="3" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="F454" s="3" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="G454" s="3" t="s">
         <v>37</v>
       </c>
       <c r="H454" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I454" s="4" t="s">
         <v>17</v>
@@ -20374,16 +20372,16 @@
         <v>66</v>
       </c>
       <c r="E455" s="5" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="F455" s="5" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="G455" s="5" t="s">
         <v>22</v>
       </c>
       <c r="H455" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I455" s="6" t="s">
         <v>17</v>
@@ -20406,16 +20404,16 @@
         <v>67</v>
       </c>
       <c r="E456" s="3" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="F456" s="3" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="G456" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H456" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I456" s="4" t="s">
         <v>17</v>
@@ -20438,16 +20436,16 @@
         <v>68</v>
       </c>
       <c r="E457" s="5" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="F457" s="5" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="G457" s="5" t="s">
         <v>22</v>
       </c>
       <c r="H457" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I457" s="6" t="s">
         <v>17</v>
@@ -20470,16 +20468,16 @@
         <v>69</v>
       </c>
       <c r="E458" s="3" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="F458" s="3" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="G458" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H458" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I458" s="4" t="s">
         <v>17</v>
@@ -20502,16 +20500,16 @@
         <v>70</v>
       </c>
       <c r="E459" s="5" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="F459" s="5" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="G459" s="5" t="s">
         <v>37</v>
       </c>
       <c r="H459" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I459" s="6" t="s">
         <v>17</v>
@@ -20534,16 +20532,16 @@
         <v>31</v>
       </c>
       <c r="E460" s="3" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="F460" s="3" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="G460" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H460" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I460" s="4" t="s">
         <v>17</v>
@@ -20566,16 +20564,16 @@
         <v>32</v>
       </c>
       <c r="E461" s="5" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="F461" s="5" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="G461" s="5" t="s">
         <v>22</v>
       </c>
       <c r="H461" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I461" s="6" t="s">
         <v>17</v>
@@ -20598,16 +20596,16 @@
         <v>33</v>
       </c>
       <c r="E462" s="3" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="F462" s="3" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="G462" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H462" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I462" s="4" t="s">
         <v>17</v>
@@ -20635,7 +20633,7 @@
         <v>22</v>
       </c>
       <c r="H463" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I463" s="6" t="s">
         <v>114</v>
@@ -20660,26 +20658,26 @@
         <v>35</v>
       </c>
       <c r="E464" s="3" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="F464" s="3" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="G464" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H464" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I464" s="4" t="s">
         <v>17</v>
       </c>
       <c r="J464" s="4"/>
       <c r="K464" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="L464" s="7" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
     </row>
     <row r="465" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
@@ -20696,16 +20694,16 @@
         <v>36</v>
       </c>
       <c r="E465" s="5" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="F465" s="5" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="G465" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H465" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I465" s="6" t="s">
         <v>17</v>
@@ -20728,16 +20726,16 @@
         <v>37</v>
       </c>
       <c r="E466" s="3" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="F466" s="3" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="G466" s="3" t="s">
         <v>32</v>
       </c>
       <c r="H466" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I466" s="4" t="s">
         <v>17</v>
@@ -20765,13 +20763,13 @@
         <v>22</v>
       </c>
       <c r="H467" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I467" s="6" t="s">
         <v>114</v>
       </c>
       <c r="J467" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="K467" s="6"/>
       <c r="L467" s="6"/>
@@ -20795,7 +20793,7 @@
         <v>22</v>
       </c>
       <c r="H468" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I468" s="4" t="s">
         <v>114</v>
@@ -20825,7 +20823,7 @@
         <v>37</v>
       </c>
       <c r="H469" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="I469" s="6" t="s">
         <v>114</v>

</xml_diff>